<commit_message>
Se añadio el campo Descripción a la Tabla de Equivalencias del Modulo Gestionar Producto
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M3.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB0ECE3B-B011-4637-9EE4-3F0E22170014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C70270-7F3D-4859-834D-03B6499119DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -143,13 +143,96 @@
   </si>
   <si>
     <t>CENV&lt;03&gt;</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>Lógico</t>
+  </si>
+  <si>
+    <t>Descripción= caracteres alfanuméricos</t>
+  </si>
+  <si>
+    <t>CEV&lt;02&gt;</t>
+  </si>
+  <si>
+    <t>Descripción!= caracteres alfanuméricos</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;04&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>1 &lt; Descripción&lt;= 50</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;03&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Descripción&lt;= 1</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;05&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Descripción&gt; 50</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;06&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -200,6 +283,12 @@
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF993300"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -398,7 +487,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -490,30 +579,45 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -799,7 +903,7 @@
   <dimension ref="B1:G1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -818,14 +922,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="31" t="s">
+      <c r="E3" s="34"/>
+      <c r="F3" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="32"/>
+      <c r="G3" s="34"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -848,52 +952,99 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="F5" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="G5" s="31" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="38" t="s">
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="38" t="s">
+      <c r="G6" s="32" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="38" t="s">
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="38" t="s">
+      <c r="G7" s="32" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="2:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="2:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="36"/>
+      <c r="C9" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="44" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="44" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="11" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1887,7 +2038,11 @@
     <row r="1001" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="10">
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="B5:B7"/>
@@ -1923,20 +2078,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="32"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="34"/>
     </row>
     <row r="3" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
@@ -1966,11 +2121,11 @@
       <c r="I3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="35" t="s">
+      <c r="J3" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="36"/>
-      <c r="L3" s="32"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="34"/>
     </row>
     <row r="4" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">

</xml_diff>

<commit_message>
Se añadio el campo Stock a la Tabla de Equivalencias del Modulo Gestionar Producto
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M3.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C70270-7F3D-4859-834D-03B6499119DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A19F8AE-34FA-48A1-8CB9-1A627CDF73E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -226,6 +226,33 @@
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>0&lt;=Stock&lt;=999999999</t>
+  </si>
+  <si>
+    <t>CEV&lt;04&gt;</t>
+  </si>
+  <si>
+    <t>Stock!= caracteres numéricos</t>
+  </si>
+  <si>
+    <t>CENV&lt;07&gt;</t>
+  </si>
+  <si>
+    <t>Stock&gt;999999999</t>
+  </si>
+  <si>
+    <t>CENV&lt;08&gt;</t>
+  </si>
+  <si>
+    <t>Stock&lt; 0</t>
+  </si>
+  <si>
+    <t>CENV&lt;09&gt;</t>
   </si>
 </sst>
 </file>
@@ -585,40 +612,40 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -903,7 +930,7 @@
   <dimension ref="B1:G1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B11" sqref="B11:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -922,14 +949,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="34"/>
-      <c r="F3" s="33" t="s">
+      <c r="E3" s="42"/>
+      <c r="F3" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="34"/>
+      <c r="G3" s="42"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -952,16 +979,16 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="36" t="s">
         <v>32</v>
       </c>
       <c r="F5" s="31" t="s">
@@ -972,10 +999,10 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
       <c r="F6" s="32" t="s">
         <v>35</v>
       </c>
@@ -984,10 +1011,10 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
       <c r="F7" s="32" t="s">
         <v>37</v>
       </c>
@@ -996,58 +1023,99 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="43" t="s">
+      <c r="D8" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="43" t="s">
+      <c r="E8" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="43" t="s">
+      <c r="F8" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="43" t="s">
+      <c r="G8" s="34" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="36"/>
-      <c r="C9" s="35" t="s">
+      <c r="B9" s="37"/>
+      <c r="C9" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="45" t="s">
+      <c r="D9" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="E9" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="44" t="s">
+      <c r="F9" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="44" t="s">
+      <c r="G9" s="35" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="44" t="s">
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="44" t="s">
+      <c r="G10" s="35" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" s="32" t="s">
+        <v>60</v>
+      </c>
+    </row>
     <row r="14" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="16" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2038,17 +2106,21 @@
     <row r="1001" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="14">
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -2078,20 +2150,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="34"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="42"/>
     </row>
     <row r="3" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
@@ -2121,11 +2193,11 @@
       <c r="I3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="40" t="s">
+      <c r="J3" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="41"/>
-      <c r="L3" s="34"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="42"/>
     </row>
     <row r="4" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">

</xml_diff>

<commit_message>
Se añadio el campo Nombre categoria descripcion a la Tabla de Equivalencias del Modulo Gestionar Producto
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M3.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A19F8AE-34FA-48A1-8CB9-1A627CDF73E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D89F24-F1A7-433C-B8A6-9E8FC57DFE16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="67">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -254,12 +254,63 @@
   <si>
     <t>CENV&lt;09&gt;</t>
   </si>
+  <si>
+    <t>Nombre categoria descripcion</t>
+  </si>
+  <si>
+    <r>
+      <t>Miembro de un Conjunto</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Nombre categoria descripcion=Opción Disponible</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;05&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Nombre rol descripcion= NULL</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;06&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -318,6 +369,13 @@
       <color rgb="FF993300"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -514,7 +572,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -630,22 +688,31 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -675,8 +742,8 @@
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>638175</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -930,7 +997,7 @@
   <dimension ref="B1:G1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:B13"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -949,14 +1016,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="41" t="s">
+      <c r="E3" s="40"/>
+      <c r="F3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="42"/>
+      <c r="G3" s="40"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -1047,10 +1114,10 @@
       <c r="C9" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="39" t="s">
+      <c r="D9" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="39" t="s">
+      <c r="E9" s="41" t="s">
         <v>47</v>
       </c>
       <c r="F9" s="35" t="s">
@@ -1063,8 +1130,8 @@
     <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="38"/>
       <c r="C10" s="38"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
       <c r="F10" s="35" t="s">
         <v>50</v>
       </c>
@@ -1116,9 +1183,42 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="2:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+    </row>
+    <row r="15" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+    </row>
+    <row r="16" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
+    </row>
     <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2106,7 +2206,13 @@
     <row r="1001" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="20">
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F16"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="D11:D13"/>
@@ -2163,7 +2269,7 @@
       <c r="E2" s="46"/>
       <c r="F2" s="46"/>
       <c r="G2" s="46"/>
-      <c r="H2" s="42"/>
+      <c r="H2" s="40"/>
     </row>
     <row r="3" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
@@ -2197,7 +2303,7 @@
         <v>17</v>
       </c>
       <c r="K3" s="46"/>
-      <c r="L3" s="42"/>
+      <c r="L3" s="40"/>
     </row>
     <row r="4" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">

</xml_diff>

<commit_message>
Se añadio el campo Precio a la Tabla de Equivalencias del Modulo Gestionar Producto
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M3.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D89F24-F1A7-433C-B8A6-9E8FC57DFE16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC32B57A-8251-4201-A7F7-0B5B05593408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="75">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -304,6 +304,30 @@
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
+  </si>
+  <si>
+    <t>Precio</t>
+  </si>
+  <si>
+    <t>0&lt;=Precio&lt;=999999999999999</t>
+  </si>
+  <si>
+    <t>CEV&lt;07&gt;</t>
+  </si>
+  <si>
+    <t>Precio!= caracteres numéricos</t>
+  </si>
+  <si>
+    <t>CENV&lt;10&gt;</t>
+  </si>
+  <si>
+    <t>Stock&gt;999999999999999</t>
+  </si>
+  <si>
+    <t>CENV&lt;11&gt;</t>
+  </si>
+  <si>
+    <t>CENV&lt;12&gt;</t>
   </si>
 </sst>
 </file>
@@ -679,6 +703,15 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -688,31 +721,22 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -997,7 +1021,7 @@
   <dimension ref="B1:G1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B17" sqref="B17:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1016,14 +1040,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="40"/>
-      <c r="F3" s="39" t="s">
+      <c r="E3" s="45"/>
+      <c r="F3" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="40"/>
+      <c r="G3" s="45"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -1046,16 +1070,16 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="39" t="s">
         <v>32</v>
       </c>
       <c r="F5" s="31" t="s">
@@ -1066,10 +1090,10 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
       <c r="F6" s="32" t="s">
         <v>35</v>
       </c>
@@ -1078,10 +1102,10 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
       <c r="F7" s="32" t="s">
         <v>37</v>
       </c>
@@ -1090,7 +1114,7 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="39" t="s">
         <v>39</v>
       </c>
       <c r="C8" s="33" t="s">
@@ -1110,14 +1134,14 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="37"/>
-      <c r="C9" s="36" t="s">
+      <c r="B9" s="40"/>
+      <c r="C9" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="41" t="s">
+      <c r="E9" s="42" t="s">
         <v>47</v>
       </c>
       <c r="F9" s="35" t="s">
@@ -1128,10 +1152,10 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
       <c r="F10" s="35" t="s">
         <v>50</v>
       </c>
@@ -1140,16 +1164,16 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="39" t="s">
         <v>54</v>
       </c>
       <c r="F11" s="31" t="s">
@@ -1160,10 +1184,10 @@
       </c>
     </row>
     <row r="12" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
       <c r="F12" s="32" t="s">
         <v>57</v>
       </c>
@@ -1172,10 +1196,10 @@
       </c>
     </row>
     <row r="13" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
       <c r="F13" s="32" t="s">
         <v>59</v>
       </c>
@@ -1184,57 +1208,98 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="41" t="s">
+      <c r="D14" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="41" t="s">
+      <c r="E14" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
     </row>
     <row r="15" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
     </row>
     <row r="16" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
       <c r="D16" s="35" t="s">
         <v>65</v>
       </c>
       <c r="E16" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
     </row>
-    <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" s="32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G19" s="32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2206,13 +2271,11 @@
     <row r="1001" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F16"/>
+  <mergeCells count="24">
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="E17:E19"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="D11:D13"/>
@@ -2227,6 +2290,12 @@
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="D3:E3"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -2256,20 +2325,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="40"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="45"/>
     </row>
     <row r="3" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
@@ -2299,11 +2368,11 @@
       <c r="I3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="45" t="s">
+      <c r="J3" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="46"/>
-      <c r="L3" s="40"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="45"/>
     </row>
     <row r="4" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">

</xml_diff>

<commit_message>
Se añadio el campo Fotos a la Tabla de Equivalencias del Modulo Gestionar Producto
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M3.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC32B57A-8251-4201-A7F7-0B5B05593408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80232A28-4F6F-4547-923E-CA19E02DB2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="82">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -329,12 +329,33 @@
   <si>
     <t>CENV&lt;12&gt;</t>
   </si>
+  <si>
+    <t>Fotos</t>
+  </si>
+  <si>
+    <t>Fotos = Archivo imagen</t>
+  </si>
+  <si>
+    <t>CEV&lt;08&gt;</t>
+  </si>
+  <si>
+    <t>Foto != Archivo imagen</t>
+  </si>
+  <si>
+    <t>CENV&lt;13&gt;</t>
+  </si>
+  <si>
+    <t>Fotos = Nulo</t>
+  </si>
+  <si>
+    <t>CEV&lt;09&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -396,6 +417,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -596,7 +624,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -703,6 +731,25 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -712,31 +759,24 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1021,7 +1061,7 @@
   <dimension ref="B1:G1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:G19"/>
+      <selection activeCell="B20" sqref="B20:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1040,14 +1080,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="45"/>
-      <c r="F3" s="44" t="s">
+      <c r="E3" s="40"/>
+      <c r="F3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="45"/>
+      <c r="G3" s="40"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -1070,16 +1110,16 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="36" t="s">
         <v>32</v>
       </c>
       <c r="F5" s="31" t="s">
@@ -1090,10 +1130,10 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
       <c r="F6" s="32" t="s">
         <v>35</v>
       </c>
@@ -1102,10 +1142,10 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
       <c r="F7" s="32" t="s">
         <v>37</v>
       </c>
@@ -1114,7 +1154,7 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="36" t="s">
         <v>39</v>
       </c>
       <c r="C8" s="33" t="s">
@@ -1134,14 +1174,14 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="40"/>
-      <c r="C9" s="39" t="s">
+      <c r="B9" s="37"/>
+      <c r="C9" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="41" t="s">
         <v>47</v>
       </c>
       <c r="F9" s="35" t="s">
@@ -1152,10 +1192,10 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
       <c r="F10" s="35" t="s">
         <v>50</v>
       </c>
@@ -1164,16 +1204,16 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D11" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="39" t="s">
+      <c r="E11" s="36" t="s">
         <v>54</v>
       </c>
       <c r="F11" s="31" t="s">
@@ -1184,10 +1224,10 @@
       </c>
     </row>
     <row r="12" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="32" t="s">
         <v>57</v>
       </c>
@@ -1196,10 +1236,10 @@
       </c>
     </row>
     <row r="13" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
       <c r="F13" s="32" t="s">
         <v>59</v>
       </c>
@@ -1208,52 +1248,52 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="42" t="s">
+      <c r="E14" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
     </row>
     <row r="15" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="40"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
     </row>
     <row r="16" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
       <c r="D16" s="35" t="s">
         <v>65</v>
       </c>
       <c r="E16" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
     </row>
     <row r="17" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="39" t="s">
+      <c r="D17" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="39" t="s">
+      <c r="E17" s="36" t="s">
         <v>69</v>
       </c>
       <c r="F17" s="31" t="s">
@@ -1264,10 +1304,10 @@
       </c>
     </row>
     <row r="18" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="40"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
       <c r="F18" s="32" t="s">
         <v>72</v>
       </c>
@@ -1276,10 +1316,10 @@
       </c>
     </row>
     <row r="19" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
       <c r="F19" s="32" t="s">
         <v>59</v>
       </c>
@@ -1287,9 +1327,46 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="G20" s="41" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="37"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+    </row>
+    <row r="22" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="38"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="50"/>
+      <c r="G22" s="50"/>
+    </row>
     <row r="23" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2271,7 +2348,29 @@
     <row r="1001" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="30">
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
     <mergeCell ref="B17:B19"/>
     <mergeCell ref="C17:C19"/>
     <mergeCell ref="D17:D19"/>
@@ -2280,22 +2379,6 @@
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="D11:D13"/>
     <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -2338,7 +2421,7 @@
       <c r="E2" s="49"/>
       <c r="F2" s="49"/>
       <c r="G2" s="49"/>
-      <c r="H2" s="45"/>
+      <c r="H2" s="40"/>
     </row>
     <row r="3" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
@@ -2372,7 +2455,7 @@
         <v>17</v>
       </c>
       <c r="K3" s="49"/>
-      <c r="L3" s="45"/>
+      <c r="L3" s="40"/>
     </row>
     <row r="4" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">

</xml_diff>

<commit_message>
Se añadio el campo Descripcion a la Tabla de Equivalencias del Modulo Gestionar Producto
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M3.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80232A28-4F6F-4547-923E-CA19E02DB2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97BA653-96BF-425E-B47F-91A2DAB680C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="89">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -349,6 +349,71 @@
   </si>
   <si>
     <t>CEV&lt;09&gt;</t>
+  </si>
+  <si>
+    <t>CEV&lt;10&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;14&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>1 &lt; Descripción&lt;= 500</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;11&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;15&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Descripción&gt; 500</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;16&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF993300"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -731,6 +796,15 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -740,43 +814,34 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1061,7 +1126,7 @@
   <dimension ref="B1:G1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:G22"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1080,14 +1145,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="40"/>
-      <c r="F3" s="39" t="s">
+      <c r="E3" s="49"/>
+      <c r="F3" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="40"/>
+      <c r="G3" s="49"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -1110,16 +1175,16 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="39" t="s">
         <v>32</v>
       </c>
       <c r="F5" s="31" t="s">
@@ -1130,10 +1195,10 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
       <c r="F6" s="32" t="s">
         <v>35</v>
       </c>
@@ -1142,10 +1207,10 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
       <c r="F7" s="32" t="s">
         <v>37</v>
       </c>
@@ -1154,7 +1219,7 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="39" t="s">
         <v>39</v>
       </c>
       <c r="C8" s="33" t="s">
@@ -1174,14 +1239,14 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="37"/>
-      <c r="C9" s="36" t="s">
+      <c r="B9" s="40"/>
+      <c r="C9" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="41" t="s">
+      <c r="E9" s="37" t="s">
         <v>47</v>
       </c>
       <c r="F9" s="35" t="s">
@@ -1192,10 +1257,10 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
       <c r="F10" s="35" t="s">
         <v>50</v>
       </c>
@@ -1204,16 +1269,16 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="39" t="s">
         <v>54</v>
       </c>
       <c r="F11" s="31" t="s">
@@ -1224,10 +1289,10 @@
       </c>
     </row>
     <row r="12" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
       <c r="F12" s="32" t="s">
         <v>57</v>
       </c>
@@ -1236,10 +1301,10 @@
       </c>
     </row>
     <row r="13" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
       <c r="F13" s="32" t="s">
         <v>59</v>
       </c>
@@ -1248,52 +1313,52 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="41" t="s">
+      <c r="D14" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="41" t="s">
+      <c r="E14" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
     </row>
     <row r="15" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
     </row>
     <row r="16" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
       <c r="D16" s="35" t="s">
         <v>65</v>
       </c>
       <c r="E16" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
     </row>
     <row r="17" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="36" t="s">
+      <c r="C17" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="36" t="s">
+      <c r="D17" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="36" t="s">
+      <c r="E17" s="39" t="s">
         <v>69</v>
       </c>
       <c r="F17" s="31" t="s">
@@ -1304,10 +1369,10 @@
       </c>
     </row>
     <row r="18" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
       <c r="F18" s="32" t="s">
         <v>72</v>
       </c>
@@ -1316,10 +1381,10 @@
       </c>
     </row>
     <row r="19" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
       <c r="F19" s="32" t="s">
         <v>59</v>
       </c>
@@ -1328,48 +1393,95 @@
       </c>
     </row>
     <row r="20" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="51" t="s">
+      <c r="C20" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="41" t="s">
+      <c r="D20" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="E20" s="41" t="s">
+      <c r="E20" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="F20" s="41" t="s">
+      <c r="F20" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="G20" s="41" t="s">
+      <c r="G20" s="37" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="37"/>
-      <c r="C21" s="52"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
     </row>
     <row r="22" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="38"/>
-      <c r="C22" s="53"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="44"/>
       <c r="D22" s="35" t="s">
         <v>80</v>
       </c>
       <c r="E22" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="F22" s="50"/>
-      <c r="G22" s="50"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
     </row>
-    <row r="23" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="G23" s="34" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="40"/>
+      <c r="C24" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="F24" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24" s="35" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="G25" s="35" t="s">
+        <v>88</v>
+      </c>
+    </row>
     <row r="26" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2348,29 +2460,11 @@
     <row r="1001" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
+  <mergeCells count="34">
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
     <mergeCell ref="B17:B19"/>
     <mergeCell ref="C17:C19"/>
     <mergeCell ref="D17:D19"/>
@@ -2379,6 +2473,28 @@
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="D11:D13"/>
     <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -2408,20 +2524,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="40"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="49"/>
     </row>
     <row r="3" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
@@ -2451,11 +2567,11 @@
       <c r="I3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="48" t="s">
+      <c r="J3" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="49"/>
-      <c r="L3" s="40"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="49"/>
     </row>
     <row r="4" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">

</xml_diff>

<commit_message>
Se añadio Los casos de Prueba para entradas correctas CP1 y CP2 no se reportaron errores
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M3.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97BA653-96BF-425E-B47F-91A2DAB680C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2FCF36-2EA7-4326-8654-64A93E2AB961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clases de equivalencia Nuevo Pr" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="98">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -46,34 +46,13 @@
     <t>Código</t>
   </si>
   <si>
-    <t>AGREGAR USUARIO</t>
-  </si>
-  <si>
     <t>CONDICIONES DE ENTRADA</t>
   </si>
   <si>
     <t>Caso prueba</t>
   </si>
   <si>
-    <t xml:space="preserve">Escenario </t>
-  </si>
-  <si>
     <t>Clases de equivalencia</t>
-  </si>
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Usuario</t>
-  </si>
-  <si>
-    <t>Contraseña</t>
-  </si>
-  <si>
-    <t>Tipo de Perfil</t>
-  </si>
-  <si>
-    <t>Foto</t>
   </si>
   <si>
     <t>Resultado esperado</t>
@@ -415,12 +394,60 @@
       <t xml:space="preserve"> </t>
     </r>
   </si>
+  <si>
+    <t>Observaciones</t>
+  </si>
+  <si>
+    <t>Nuevo Producto</t>
+  </si>
+  <si>
+    <t>Escenario</t>
+  </si>
+  <si>
+    <t>Obseraciones</t>
+  </si>
+  <si>
+    <t>Registro Exitroso</t>
+  </si>
+  <si>
+    <t>CEV&lt;01&gt;,CEV&lt;02&gt;,CEV&lt;04&gt;,CEV&lt;05&gt;,CEV&lt;07&gt;,CEV&lt;08&gt;,CEV&lt;10&gt;</t>
+  </si>
+  <si>
+    <t>Cartera de cuero</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>Imagen Jpg</t>
+  </si>
+  <si>
+    <t>De buena calidad</t>
+  </si>
+  <si>
+    <t>Se Registra correctamente el Producto</t>
+  </si>
+  <si>
+    <t>Se registra y se muestra el mensaje: "Producto creado/a satisfactoriamente"</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>CEV&lt;01&gt;, CEV&lt;03&gt; ,CEV&lt;04&gt;,CEV&lt;06&gt;,CEV&lt;07&gt; ,CEV&lt;09&gt;,CEV&lt;11&gt;</t>
+  </si>
+  <si>
+    <t>Cinturón de cuero</t>
+  </si>
+  <si>
+    <t>Importada</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -494,8 +521,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -506,12 +546,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
         <bgColor rgb="FFFFFF99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDAEEF3"/>
-        <bgColor rgb="FFDAEEF3"/>
       </patternFill>
     </fill>
     <fill>
@@ -544,8 +578,20 @@
         <bgColor rgb="FF9FC5E8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDAEEF3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -608,17 +654,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
@@ -685,11 +720,93 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -700,11 +817,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -712,15 +826,12 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -769,79 +880,102 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -904,6 +1038,72 @@
         <a:xfrm>
           <a:off x="7800975" y="152400"/>
           <a:ext cx="7810500" cy="6353175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>409575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BC57570-89C8-0C30-4C79-18288EB01781}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15563850" y="762000"/>
+          <a:ext cx="2647950" cy="409575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1125,8 +1325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1145,14 +1345,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="49"/>
-      <c r="F3" s="48" t="s">
+      <c r="E3" s="37"/>
+      <c r="F3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="49"/>
+      <c r="G3" s="37"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -1175,311 +1375,311 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="31" t="s">
-        <v>34</v>
+      <c r="C5" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="32" t="s">
-        <v>36</v>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="32" t="s">
-        <v>38</v>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="39" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" s="34" t="s">
-        <v>44</v>
+      <c r="B8" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="40"/>
-      <c r="C9" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" s="35" t="s">
-        <v>49</v>
+      <c r="B9" s="32"/>
+      <c r="C9" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="29" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" s="35" t="s">
-        <v>51</v>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="G11" s="31" t="s">
-        <v>56</v>
+      <c r="B11" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="32" t="s">
-        <v>58</v>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="G13" s="32" t="s">
-        <v>60</v>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="26" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
+      <c r="B14" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
     </row>
     <row r="15" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="40"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
     </row>
     <row r="16" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
     </row>
     <row r="17" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="F17" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="G17" s="31" t="s">
-        <v>71</v>
+      <c r="B17" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="25" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="40"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="G18" s="32" t="s">
-        <v>73</v>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" s="26" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="G19" s="32" t="s">
-        <v>74</v>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19" s="26" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="E20" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="F20" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="G20" s="37" t="s">
-        <v>79</v>
+      <c r="B20" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" s="34" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="40"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
     </row>
     <row r="22" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="41"/>
-      <c r="C22" s="44"/>
-      <c r="D22" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="E22" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
     </row>
     <row r="23" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="39" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="34" t="s">
+      <c r="B23" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="F23" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="G23" s="34" t="s">
-        <v>83</v>
+      <c r="C23" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G23" s="28" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="40"/>
-      <c r="C24" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="E24" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="F24" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="G24" s="35" t="s">
-        <v>86</v>
+      <c r="B24" s="32"/>
+      <c r="C24" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="F24" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="G24" s="29" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="41"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="G25" s="35" t="s">
-        <v>88</v>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="G25" s="29" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2461,14 +2661,18 @@
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F16"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="D11:D13"/>
@@ -2483,18 +2687,14 @@
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="E17:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -2504,10 +2704,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L991"/>
+  <dimension ref="A1:Q991"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2519,250 +2719,333 @@
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
     <col min="7" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="25.42578125" customWidth="1"/>
-    <col min="10" max="28" width="10" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" customWidth="1"/>
+    <col min="12" max="28" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="50" t="s">
+    <row r="1" spans="1:17" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+    </row>
+    <row r="2" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
     </row>
-    <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="52" t="s">
+    <row r="3" spans="1:17" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="49"/>
+      <c r="B3" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="J3" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="K3" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="50"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="49" t="s">
+        <v>85</v>
+      </c>
+      <c r="P3" s="50"/>
+      <c r="Q3" s="51"/>
     </row>
-    <row r="3" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4" t="s">
+    <row r="4" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="53">
+        <v>5</v>
+      </c>
+      <c r="E4" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="53">
         <v>10</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="G4" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" s="53">
+        <v>50</v>
+      </c>
+      <c r="I4" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="J4" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="K4" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="L4" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="M4" s="57"/>
+      <c r="N4" s="58"/>
+      <c r="O4" s="56" t="s">
+        <v>94</v>
+      </c>
+      <c r="P4" s="57"/>
+      <c r="Q4" s="58"/>
+    </row>
+    <row r="5" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="B5" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="55" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="55">
+        <v>111</v>
+      </c>
+      <c r="E5" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" s="55">
+        <v>45</v>
+      </c>
+      <c r="G5" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" s="55">
+        <v>10</v>
+      </c>
+      <c r="I5" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="J5" s="55" t="s">
+        <v>97</v>
+      </c>
+      <c r="K5" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="L5" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="M5" s="57"/>
+      <c r="N5" s="58"/>
+      <c r="O5" s="56" t="s">
+        <v>94</v>
+      </c>
+      <c r="P5" s="57"/>
+      <c r="Q5" s="58"/>
+    </row>
+    <row r="6" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="52" t="s">
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="53"/>
-      <c r="L3" s="49"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
     </row>
-    <row r="4" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+    <row r="11" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
     </row>
-    <row r="5" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+    <row r="12" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
     </row>
-    <row r="6" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
+    <row r="13" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
     </row>
-    <row r="7" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+    <row r="14" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
     </row>
-    <row r="8" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
+    <row r="15" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="22"/>
     </row>
-    <row r="9" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-    </row>
-    <row r="10" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-    </row>
-    <row r="11" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-    </row>
-    <row r="12" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-    </row>
-    <row r="13" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-    </row>
-    <row r="14" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-    </row>
-    <row r="15" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="28"/>
-    </row>
-    <row r="16" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3739,12 +4022,18 @@
     <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="8">
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="O5:Q5"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="L3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se añadio Los casos de Prueba para entradas Código incorrectas no se reportaron errores
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M3.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2FCF36-2EA7-4326-8654-64A93E2AB961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6819D4F-D0F4-4C01-913F-231D7B428712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="113">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -442,12 +442,90 @@
   <si>
     <t>Importada</t>
   </si>
+  <si>
+    <t>Registro con Código Incorrecto</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;01&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, CEV&lt;03&gt; ,CEV&lt;04&gt;,CEV&lt;06&gt;,CEV&lt;07&gt; ,CEV&lt;09&gt;,CEV&lt;11&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>/*/</t>
+  </si>
+  <si>
+    <t>Bolso de cuero</t>
+  </si>
+  <si>
+    <t>De marca</t>
+  </si>
+  <si>
+    <t>No se permite el Registro</t>
+  </si>
+  <si>
+    <t>No se permite el ingreso de "/*/" como Código</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;02&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, CEV&lt;03&gt; ,CEV&lt;04&gt;,CEV&lt;06&gt;,CEV&lt;07&gt; ,CEV&lt;09&gt;,CEV&lt;11&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Chaqueta de cuero</t>
+  </si>
+  <si>
+    <t>Producto nacional</t>
+  </si>
+  <si>
+    <t>No se permite el ingreso de "9999...." como Código</t>
+  </si>
+  <si>
+    <r>
+      <t>CENV&lt;03&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, CEV&lt;03&gt; ,CEV&lt;04&gt;,CEV&lt;06&gt;,CEV&lt;07&gt; ,CEV&lt;09&gt;,CEV&lt;11&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Zapato de cuero</t>
+  </si>
+  <si>
+    <t>Edición especial</t>
+  </si>
+  <si>
+    <t>No se permite el Registro y se muestra el Mensaje: "Es obligado que Código en Producto tenga valor"</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -534,6 +612,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -546,12 +630,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
         <bgColor rgb="FFFFFF99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB6D7A8"/>
-        <bgColor rgb="FFB6D7A8"/>
       </patternFill>
     </fill>
     <fill>
@@ -590,6 +668,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB6D7A8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -806,7 +890,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -868,18 +952,6 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -898,6 +970,33 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -907,73 +1006,64 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1104,6 +1194,67 @@
         <a:xfrm>
           <a:off x="15563850" y="762000"/>
           <a:ext cx="2647950" cy="409575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>542925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46FDB00D-445F-B3FA-AD89-914E911D1E13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15668625" y="3800475"/>
+          <a:ext cx="3171825" cy="476250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1345,14 +1496,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="36" t="s">
+      <c r="E3" s="46"/>
+      <c r="F3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="37"/>
+      <c r="G3" s="46"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -1375,72 +1526,72 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="G5" s="21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="26" t="s">
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="26" t="s">
+      <c r="G6" s="22" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="26" t="s">
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="22" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="24" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="32"/>
-      <c r="C9" s="31" t="s">
+      <c r="B9" s="37"/>
+      <c r="C9" s="36" t="s">
         <v>38</v>
       </c>
       <c r="D9" s="34" t="s">
@@ -1449,74 +1600,74 @@
       <c r="E9" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="29" t="s">
+      <c r="F9" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="25" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
       <c r="D10" s="35"/>
       <c r="E10" s="35"/>
-      <c r="F10" s="29" t="s">
+      <c r="F10" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="G10" s="29" t="s">
+      <c r="G10" s="25" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="G11" s="25" t="s">
+      <c r="G11" s="21" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="26" t="s">
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="G12" s="26" t="s">
+      <c r="G12" s="22" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="26" t="s">
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="26" t="s">
+      <c r="G13" s="22" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="36" t="s">
         <v>55</v>
       </c>
       <c r="D14" s="34" t="s">
@@ -1525,78 +1676,78 @@
       <c r="E14" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
     </row>
     <row r="15" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
       <c r="D15" s="35"/>
       <c r="E15" s="35"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
     </row>
     <row r="16" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="29" t="s">
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="29" t="s">
+      <c r="E16" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
     </row>
     <row r="17" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="E17" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="25" t="s">
+      <c r="F17" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="G17" s="25" t="s">
+      <c r="G17" s="21" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="26" t="s">
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="G18" s="26" t="s">
+      <c r="G18" s="22" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="26" t="s">
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="26" t="s">
+      <c r="G19" s="22" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="41" t="s">
+      <c r="C20" s="39" t="s">
         <v>33</v>
       </c>
       <c r="D20" s="34" t="s">
@@ -1613,48 +1764,48 @@
       </c>
     </row>
     <row r="21" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="32"/>
-      <c r="C21" s="42"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="40"/>
       <c r="D21" s="35"/>
       <c r="E21" s="35"/>
       <c r="F21" s="35"/>
       <c r="G21" s="35"/>
     </row>
     <row r="22" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="33"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="29" t="s">
+      <c r="B22" s="38"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="E22" s="29" t="s">
+      <c r="E22" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
     </row>
     <row r="23" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="27" t="s">
+      <c r="C23" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="28" t="s">
+      <c r="E23" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="F23" s="28" t="s">
+      <c r="F23" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="G23" s="28" t="s">
+      <c r="G23" s="24" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="32"/>
-      <c r="C24" s="31" t="s">
+      <c r="B24" s="37"/>
+      <c r="C24" s="36" t="s">
         <v>38</v>
       </c>
       <c r="D24" s="34" t="s">
@@ -1663,22 +1814,22 @@
       <c r="E24" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="F24" s="29" t="s">
+      <c r="F24" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="G24" s="29" t="s">
+      <c r="G24" s="25" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
       <c r="D25" s="35"/>
       <c r="E25" s="35"/>
-      <c r="F25" s="29" t="s">
+      <c r="F25" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="G25" s="29" t="s">
+      <c r="G25" s="25" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2661,18 +2812,14 @@
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="E17:E19"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="D11:D13"/>
@@ -2687,14 +2834,18 @@
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -2707,7 +2858,7 @@
   <dimension ref="A1:Q991"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2726,324 +2877,411 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="49" t="s">
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
     </row>
     <row r="3" spans="1:17" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="48" t="s">
+      <c r="E3" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="48" t="s">
+      <c r="G3" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="48" t="s">
+      <c r="H3" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="I3" s="48" t="s">
+      <c r="I3" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="J3" s="48" t="s">
+      <c r="J3" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="K3" s="48" t="s">
+      <c r="K3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="49" t="s">
+      <c r="L3" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="50"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="49" t="s">
+      <c r="M3" s="48"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="51"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="49"/>
     </row>
     <row r="4" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="53">
+      <c r="D4" s="31">
         <v>5</v>
       </c>
-      <c r="E4" s="53" t="s">
+      <c r="E4" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="F4" s="53">
+      <c r="F4" s="31">
         <v>10</v>
       </c>
-      <c r="G4" s="53" t="s">
+      <c r="G4" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="H4" s="53">
+      <c r="H4" s="31">
         <v>50</v>
       </c>
-      <c r="I4" s="53" t="s">
+      <c r="I4" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="J4" s="53" t="s">
+      <c r="J4" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="K4" s="53" t="s">
+      <c r="K4" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="L4" s="56" t="s">
+      <c r="L4" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="M4" s="57"/>
-      <c r="N4" s="58"/>
-      <c r="O4" s="56" t="s">
+      <c r="M4" s="51"/>
+      <c r="N4" s="52"/>
+      <c r="O4" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="P4" s="57"/>
-      <c r="Q4" s="58"/>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="52"/>
     </row>
     <row r="5" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="55">
+      <c r="D5" s="33">
         <v>111</v>
       </c>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="F5" s="55">
+      <c r="F5" s="33">
         <v>45</v>
       </c>
-      <c r="G5" s="55" t="s">
+      <c r="G5" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="H5" s="55">
+      <c r="H5" s="33">
         <v>10</v>
       </c>
-      <c r="I5" s="55" t="s">
+      <c r="I5" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="J5" s="55" t="s">
+      <c r="J5" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="K5" s="55" t="s">
+      <c r="K5" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="L5" s="56" t="s">
+      <c r="L5" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="M5" s="57"/>
-      <c r="N5" s="58"/>
-      <c r="O5" s="56" t="s">
+      <c r="M5" s="51"/>
+      <c r="N5" s="52"/>
+      <c r="O5" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="P5" s="57"/>
-      <c r="Q5" s="58"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="52"/>
     </row>
-    <row r="6" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
+      <c r="B6" s="56" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="56" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="56" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" s="56">
+        <v>784</v>
+      </c>
+      <c r="G6" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6" s="56">
+        <v>51</v>
+      </c>
+      <c r="I6" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="J6" s="56" t="s">
+        <v>102</v>
+      </c>
+      <c r="K6" s="56" t="s">
+        <v>103</v>
+      </c>
+      <c r="L6" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="M6" s="51"/>
+      <c r="N6" s="52"/>
+      <c r="O6" s="50" t="s">
+        <v>94</v>
+      </c>
+      <c r="P6" s="51"/>
+      <c r="Q6" s="52"/>
     </row>
-    <row r="7" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
+      <c r="B7" s="59" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="60" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="59">
+        <v>9.9999999999999903E+46</v>
+      </c>
+      <c r="E7" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="59">
+        <v>64152</v>
+      </c>
+      <c r="G7" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" s="59">
+        <v>10</v>
+      </c>
+      <c r="I7" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="J7" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="K7" s="59" t="s">
+        <v>103</v>
+      </c>
+      <c r="L7" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="M7" s="51"/>
+      <c r="N7" s="52"/>
+      <c r="O7" s="50" t="s">
+        <v>94</v>
+      </c>
+      <c r="P7" s="51"/>
+      <c r="Q7" s="52"/>
     </row>
-    <row r="8" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
+      <c r="B8" s="59" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="59">
+        <v>0</v>
+      </c>
+      <c r="E8" s="59" t="s">
+        <v>110</v>
+      </c>
+      <c r="F8" s="59">
+        <v>145</v>
+      </c>
+      <c r="G8" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="59">
+        <v>21</v>
+      </c>
+      <c r="I8" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="J8" s="59" t="s">
+        <v>111</v>
+      </c>
+      <c r="K8" s="59" t="s">
+        <v>103</v>
+      </c>
+      <c r="L8" s="50" t="s">
+        <v>112</v>
+      </c>
+      <c r="M8" s="51"/>
+      <c r="N8" s="52"/>
+      <c r="O8" s="50" t="s">
+        <v>94</v>
+      </c>
+      <c r="P8" s="51"/>
+      <c r="Q8" s="52"/>
     </row>
     <row r="9" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
     </row>
     <row r="10" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
     </row>
     <row r="11" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
     </row>
     <row r="12" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
     </row>
     <row r="13" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="18"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="14"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
     </row>
     <row r="15" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="22"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="18"/>
     </row>
     <row r="16" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4022,15 +4260,21 @@
     <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="14">
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="O6:Q6"/>
     <mergeCell ref="O3:Q3"/>
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="O4:Q4"/>
     <mergeCell ref="L5:N5"/>
     <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="L3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Se añadio Los casos de Prueba para entradas Descripcion incorrectas se reporta errores en el CP06 y CP07
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M3.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6819D4F-D0F4-4C01-913F-231D7B428712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8897BC9-5C83-42C0-8F76-88D81163A20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="126">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -520,12 +520,111 @@
   <si>
     <t>No se permite el Registro y se muestra el Mensaje: "Es obligado que Código en Producto tenga valor"</t>
   </si>
+  <si>
+    <t>Registro con Descripción Incorrecto</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CEV&lt;01&gt;, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;04&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ,CEV&lt;04&gt;,CEV&lt;06&gt;,CEV&lt;07&gt; ,CEV&lt;09&gt;,CEV&lt;11&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>//&lt;&lt;x</t>
+  </si>
+  <si>
+    <t>Edición limitada</t>
+  </si>
+  <si>
+    <t>Error no se deben admitir carácteres no alfanuméricos como Descripción</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CEV&lt;01&gt;, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;05&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">,CEV&lt;04&gt;,CEV&lt;06&gt;,CEV&lt;07&gt; ,CEV&lt;09&gt;,CEV&lt;11&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Marca Nacional</t>
+  </si>
+  <si>
+    <t>Error no se deben admitir Descripción de una letra</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> CENV&lt;06&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ,CEV&lt;04&gt;,CEV&lt;06&gt;,CEV&lt;07&gt; ,CEV&lt;09&gt;,CEV&lt;11&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>gdsgegegsdgvdsgbdsgdsgsdgegegsdgfdhfdhdfhdfhdfhdsfhgshsdgfdsgsdhdshsdhsdgfds</t>
+  </si>
+  <si>
+    <t>Cuero Importado</t>
+  </si>
+  <si>
+    <t>No se permite el ingreso de "gdsgegegsdgvdsgbdsg,,,,," como Descripción</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -618,8 +717,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -630,12 +736,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
         <bgColor rgb="FFFFFF99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB4A7D6"/>
-        <bgColor rgb="FFB4A7D6"/>
       </patternFill>
     </fill>
     <fill>
@@ -674,6 +774,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4A7D6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -890,7 +1002,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -940,18 +1052,6 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -973,10 +1073,22 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -985,26 +1097,45 @@
     <xf numFmtId="0" fontId="14" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1015,28 +1146,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1048,22 +1157,34 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1496,14 +1617,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="46"/>
-      <c r="F3" s="45" t="s">
+      <c r="E3" s="42"/>
+      <c r="F3" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="46"/>
+      <c r="G3" s="42"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -1538,10 +1659,10 @@
       <c r="E5" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="17" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1550,10 +1671,10 @@
       <c r="C6" s="37"/>
       <c r="D6" s="37"/>
       <c r="E6" s="37"/>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="18" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1562,10 +1683,10 @@
       <c r="C7" s="38"/>
       <c r="D7" s="38"/>
       <c r="E7" s="38"/>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="18" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1573,19 +1694,19 @@
       <c r="B8" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="20" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1594,28 +1715,28 @@
       <c r="C9" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="D9" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="E9" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="21" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="38"/>
       <c r="C10" s="38"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="25" t="s">
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="G10" s="25" t="s">
+      <c r="G10" s="21" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1632,10 +1753,10 @@
       <c r="E11" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="17" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1644,10 +1765,10 @@
       <c r="C12" s="37"/>
       <c r="D12" s="37"/>
       <c r="E12" s="37"/>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="18" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1656,10 +1777,10 @@
       <c r="C13" s="38"/>
       <c r="D13" s="38"/>
       <c r="E13" s="38"/>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="18" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1670,34 +1791,34 @@
       <c r="C14" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="34" t="s">
+      <c r="D14" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="34" t="s">
+      <c r="E14" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
     </row>
     <row r="15" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="37"/>
       <c r="C15" s="37"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
     </row>
     <row r="16" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="38"/>
       <c r="C16" s="38"/>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
     </row>
     <row r="17" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="36" t="s">
@@ -1712,10 +1833,10 @@
       <c r="E17" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="21" t="s">
+      <c r="F17" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="G17" s="21" t="s">
+      <c r="G17" s="17" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1724,10 +1845,10 @@
       <c r="C18" s="37"/>
       <c r="D18" s="37"/>
       <c r="E18" s="37"/>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="G18" s="22" t="s">
+      <c r="G18" s="18" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1736,10 +1857,10 @@
       <c r="C19" s="38"/>
       <c r="D19" s="38"/>
       <c r="E19" s="38"/>
-      <c r="F19" s="22" t="s">
+      <c r="F19" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G19" s="18" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1747,59 +1868,59 @@
       <c r="B20" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="39" t="s">
+      <c r="C20" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="D20" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="34" t="s">
+      <c r="E20" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="F20" s="34" t="s">
+      <c r="F20" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="G20" s="34" t="s">
+      <c r="G20" s="39" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="37"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
     </row>
     <row r="22" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="38"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="25" t="s">
+      <c r="C22" s="48"/>
+      <c r="D22" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="E22" s="25" t="s">
+      <c r="E22" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
     </row>
     <row r="23" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="24" t="s">
+      <c r="D23" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="24" t="s">
+      <c r="E23" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="F23" s="24" t="s">
+      <c r="F23" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="G23" s="24" t="s">
+      <c r="G23" s="20" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1808,28 +1929,28 @@
       <c r="C24" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="34" t="s">
+      <c r="D24" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="E24" s="34" t="s">
+      <c r="E24" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="F24" s="25" t="s">
+      <c r="F24" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="G24" s="25" t="s">
+      <c r="G24" s="21" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="38"/>
       <c r="C25" s="38"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="25" t="s">
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="G25" s="25" t="s">
+      <c r="G25" s="21" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2812,14 +2933,18 @@
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F16"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="D11:D13"/>
@@ -2834,18 +2959,14 @@
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="E17:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -2857,8 +2978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q991"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2877,411 +2998,498 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="47" t="s">
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
     </row>
     <row r="3" spans="1:17" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="29" t="s">
+      <c r="H3" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="I3" s="29" t="s">
+      <c r="I3" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="J3" s="29" t="s">
+      <c r="J3" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="K3" s="29" t="s">
+      <c r="K3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="47" t="s">
+      <c r="L3" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="48"/>
-      <c r="N3" s="49"/>
-      <c r="O3" s="47" t="s">
+      <c r="M3" s="55"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="P3" s="48"/>
-      <c r="Q3" s="49"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="56"/>
     </row>
     <row r="4" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="27">
         <v>5</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="F4" s="31">
+      <c r="F4" s="27">
         <v>10</v>
       </c>
-      <c r="G4" s="31" t="s">
+      <c r="G4" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="H4" s="31">
+      <c r="H4" s="27">
         <v>50</v>
       </c>
-      <c r="I4" s="31" t="s">
+      <c r="I4" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="J4" s="31" t="s">
+      <c r="J4" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="K4" s="31" t="s">
+      <c r="K4" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="L4" s="50" t="s">
+      <c r="L4" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="M4" s="51"/>
-      <c r="N4" s="52"/>
-      <c r="O4" s="50" t="s">
+      <c r="M4" s="50"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="P4" s="51"/>
-      <c r="Q4" s="52"/>
+      <c r="P4" s="50"/>
+      <c r="Q4" s="51"/>
     </row>
     <row r="5" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="29">
         <v>111</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="29">
         <v>45</v>
       </c>
-      <c r="G5" s="33" t="s">
+      <c r="G5" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="H5" s="33">
+      <c r="H5" s="29">
         <v>10</v>
       </c>
-      <c r="I5" s="33" t="s">
+      <c r="I5" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="J5" s="33" t="s">
+      <c r="J5" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="K5" s="33" t="s">
+      <c r="K5" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="L5" s="50" t="s">
+      <c r="L5" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="M5" s="51"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="50" t="s">
+      <c r="M5" s="50"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="P5" s="51"/>
-      <c r="Q5" s="52"/>
+      <c r="P5" s="50"/>
+      <c r="Q5" s="51"/>
     </row>
     <row r="6" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="D6" s="56" t="s">
+      <c r="D6" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E6" s="56" t="s">
+      <c r="E6" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="F6" s="56">
+      <c r="F6" s="31">
         <v>784</v>
       </c>
-      <c r="G6" s="56" t="s">
+      <c r="G6" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="H6" s="56">
+      <c r="H6" s="31">
         <v>51</v>
       </c>
-      <c r="I6" s="56" t="s">
+      <c r="I6" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="J6" s="56" t="s">
+      <c r="J6" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="K6" s="56" t="s">
+      <c r="K6" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="L6" s="50" t="s">
+      <c r="L6" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="M6" s="51"/>
-      <c r="N6" s="52"/>
-      <c r="O6" s="50" t="s">
+      <c r="M6" s="50"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="P6" s="51"/>
-      <c r="Q6" s="52"/>
+      <c r="P6" s="50"/>
+      <c r="Q6" s="51"/>
     </row>
     <row r="7" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="C7" s="60" t="s">
+      <c r="C7" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="D7" s="59">
+      <c r="D7" s="34">
         <v>9.9999999999999903E+46</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="E7" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="59">
+      <c r="F7" s="34">
         <v>64152</v>
       </c>
-      <c r="G7" s="59" t="s">
+      <c r="G7" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="H7" s="59">
+      <c r="H7" s="34">
         <v>10</v>
       </c>
-      <c r="I7" s="59" t="s">
+      <c r="I7" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="J7" s="59" t="s">
+      <c r="J7" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="K7" s="59" t="s">
+      <c r="K7" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="L7" s="50" t="s">
+      <c r="L7" s="49" t="s">
         <v>108</v>
       </c>
-      <c r="M7" s="51"/>
-      <c r="N7" s="52"/>
-      <c r="O7" s="50" t="s">
+      <c r="M7" s="50"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="P7" s="51"/>
-      <c r="Q7" s="52"/>
+      <c r="P7" s="50"/>
+      <c r="Q7" s="51"/>
     </row>
     <row r="8" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="58" t="s">
+      <c r="A8" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="C8" s="60" t="s">
+      <c r="C8" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="D8" s="59">
+      <c r="D8" s="34">
         <v>0</v>
       </c>
-      <c r="E8" s="59" t="s">
+      <c r="E8" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="F8" s="59">
+      <c r="F8" s="34">
         <v>145</v>
       </c>
-      <c r="G8" s="59" t="s">
+      <c r="G8" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="H8" s="59">
+      <c r="H8" s="34">
         <v>21</v>
       </c>
-      <c r="I8" s="59" t="s">
+      <c r="I8" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="J8" s="59" t="s">
+      <c r="J8" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="K8" s="59" t="s">
+      <c r="K8" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="L8" s="50" t="s">
+      <c r="L8" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="M8" s="51"/>
-      <c r="N8" s="52"/>
-      <c r="O8" s="50" t="s">
+      <c r="M8" s="50"/>
+      <c r="N8" s="51"/>
+      <c r="O8" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="P8" s="51"/>
-      <c r="Q8" s="52"/>
+      <c r="P8" s="50"/>
+      <c r="Q8" s="51"/>
     </row>
-    <row r="9" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
+      <c r="B9" s="58" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="58" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" s="58">
+        <v>741541</v>
+      </c>
+      <c r="E9" s="58" t="s">
+        <v>115</v>
+      </c>
+      <c r="F9" s="58">
+        <v>541</v>
+      </c>
+      <c r="G9" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="58">
+        <v>41</v>
+      </c>
+      <c r="I9" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="J9" s="58" t="s">
+        <v>116</v>
+      </c>
+      <c r="K9" s="58" t="s">
+        <v>103</v>
+      </c>
+      <c r="L9" s="61" t="s">
+        <v>93</v>
+      </c>
+      <c r="M9" s="62"/>
+      <c r="N9" s="63"/>
+      <c r="O9" s="49" t="s">
+        <v>117</v>
+      </c>
+      <c r="P9" s="50"/>
+      <c r="Q9" s="51"/>
     </row>
-    <row r="10" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
+      <c r="B10" s="60" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="60" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" s="60">
+        <v>1215</v>
+      </c>
+      <c r="E10" s="60" t="s">
+        <v>119</v>
+      </c>
+      <c r="F10" s="60">
+        <v>14</v>
+      </c>
+      <c r="G10" s="60" t="s">
+        <v>89</v>
+      </c>
+      <c r="H10" s="60">
+        <v>100</v>
+      </c>
+      <c r="I10" s="60" t="s">
+        <v>89</v>
+      </c>
+      <c r="J10" s="60" t="s">
+        <v>120</v>
+      </c>
+      <c r="K10" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="L10" s="61" t="s">
+        <v>93</v>
+      </c>
+      <c r="M10" s="62"/>
+      <c r="N10" s="63"/>
+      <c r="O10" s="49" t="s">
+        <v>121</v>
+      </c>
+      <c r="P10" s="50"/>
+      <c r="Q10" s="51"/>
     </row>
-    <row r="11" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
+      <c r="B11" s="60" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="60" t="s">
+        <v>122</v>
+      </c>
+      <c r="D11" s="60">
+        <v>424</v>
+      </c>
+      <c r="E11" s="60" t="s">
+        <v>123</v>
+      </c>
+      <c r="F11" s="60">
+        <v>12541</v>
+      </c>
+      <c r="G11" s="60" t="s">
+        <v>89</v>
+      </c>
+      <c r="H11" s="60">
+        <v>115</v>
+      </c>
+      <c r="I11" s="60" t="s">
+        <v>89</v>
+      </c>
+      <c r="J11" s="60" t="s">
+        <v>124</v>
+      </c>
+      <c r="K11" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="L11" s="49" t="s">
+        <v>125</v>
+      </c>
+      <c r="M11" s="50"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="P11" s="50"/>
+      <c r="Q11" s="51"/>
     </row>
     <row r="12" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
     </row>
     <row r="13" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="14"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="10"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
     </row>
     <row r="15" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="18"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4260,7 +4468,13 @@
     <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="20">
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="O11:Q11"/>
     <mergeCell ref="L7:N7"/>
     <mergeCell ref="O7:Q7"/>
     <mergeCell ref="L8:N8"/>

</xml_diff>

<commit_message>
Se añadio Los casos de Prueba para entradas Stock incorrectas se reporta errores en el CP11
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M3.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8897BC9-5C83-42C0-8F76-88D81163A20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00D9B74-5D42-4631-9565-82F86D8FA59D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="140">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -619,12 +619,114 @@
   <si>
     <t>No se permite el ingreso de "gdsgegegsdgvdsgbdsg,,,,," como Descripción</t>
   </si>
+  <si>
+    <t>Registro con Stock Incorrecto</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;, CEV&lt;03&gt; ,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;07&gt;,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">CEV&lt;06&gt;,CEV&lt;07&gt; ,CEV&lt;09&gt;,CEV&lt;11&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Correa de reloj de cuero</t>
+  </si>
+  <si>
+    <t>bfhfdh</t>
+  </si>
+  <si>
+    <t>Cuero Nacional</t>
+  </si>
+  <si>
+    <t>No se permite el ingreso de "bfhfdh" como Stock</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;, CEV&lt;03&gt; ,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;08&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">,CEV&lt;06&gt;,CEV&lt;07&gt; ,CEV&lt;09&gt;,CEV&lt;11&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Funda de teléfono de cuero</t>
+  </si>
+  <si>
+    <t>Oferta de Temporada</t>
+  </si>
+  <si>
+    <t>No se permite el ingreso de "99999,,,," como Stock</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;, CEV&lt;03&gt; ,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;09&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">,CEV&lt;06&gt;,CEV&lt;07&gt; ,CEV&lt;09&gt;,CEV&lt;11&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Monedero de cuero</t>
+  </si>
+  <si>
+    <t>Stock Limitado</t>
+  </si>
+  <si>
+    <t>Error no se debe Permitir el ingreso de un Stock Negativo</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -644,11 +746,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -725,7 +822,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -736,18 +833,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
         <bgColor rgb="FFFFFF99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE6B8AF"/>
-        <bgColor rgb="FFE6B8AF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF9CB9C"/>
-        <bgColor rgb="FFF9CB9C"/>
       </patternFill>
     </fill>
     <fill>
@@ -786,6 +871,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4CCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -1002,7 +1093,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1013,178 +1104,163 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1617,14 +1693,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="41" t="s">
+      <c r="E3" s="43"/>
+      <c r="F3" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="42"/>
+      <c r="G3" s="43"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -1647,310 +1723,310 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="18" t="s">
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="18" t="s">
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="11" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="37"/>
-      <c r="C9" s="36" t="s">
+      <c r="B9" s="34"/>
+      <c r="C9" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="39" t="s">
+      <c r="D9" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="39" t="s">
+      <c r="E9" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="12" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="21" t="s">
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="12" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="8" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="18" t="s">
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="9" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="18" t="s">
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="G13" s="9" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="39" t="s">
+      <c r="D14" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="39" t="s">
+      <c r="E14" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
     </row>
     <row r="15" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
     </row>
     <row r="16" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="21" t="s">
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
     </row>
     <row r="17" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="36" t="s">
+      <c r="C17" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="36" t="s">
+      <c r="D17" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="36" t="s">
+      <c r="E17" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G17" s="17" t="s">
+      <c r="G17" s="8" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="18" t="s">
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="G18" s="18" t="s">
+      <c r="G18" s="9" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="18" t="s">
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="18" t="s">
+      <c r="G19" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="46" t="s">
+      <c r="C20" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="39" t="s">
+      <c r="D20" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="39" t="s">
+      <c r="E20" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="F20" s="39" t="s">
+      <c r="F20" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="G20" s="39" t="s">
+      <c r="G20" s="31" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="37"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
     </row>
     <row r="22" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="38"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="21" t="s">
+      <c r="B22" s="35"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="E22" s="21" t="s">
+      <c r="E22" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="E23" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="F23" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G23" s="20" t="s">
+      <c r="G23" s="11" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="37"/>
-      <c r="C24" s="36" t="s">
+      <c r="B24" s="34"/>
+      <c r="C24" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="39" t="s">
+      <c r="D24" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="E24" s="39" t="s">
+      <c r="E24" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="F24" s="21" t="s">
+      <c r="F24" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="G24" s="21" t="s">
+      <c r="G24" s="12" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="38"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="21" t="s">
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="G25" s="21" t="s">
+      <c r="G25" s="12" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2933,18 +3009,14 @@
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="E17:E19"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="D11:D13"/>
@@ -2959,14 +3031,18 @@
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -2978,8 +3054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q991"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13:N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2998,498 +3074,585 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="54" t="s">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
     </row>
     <row r="3" spans="1:17" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="I3" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="J3" s="25" t="s">
+      <c r="J3" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="K3" s="25" t="s">
+      <c r="K3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="54" t="s">
+      <c r="L3" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="55"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="54" t="s">
+      <c r="M3" s="53"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="56"/>
+      <c r="P3" s="53"/>
+      <c r="Q3" s="54"/>
     </row>
     <row r="4" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="18">
         <v>5</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="F4" s="27">
+      <c r="F4" s="18">
         <v>10</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="H4" s="27">
+      <c r="H4" s="18">
         <v>50</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="J4" s="27" t="s">
+      <c r="J4" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="K4" s="27" t="s">
+      <c r="K4" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="L4" s="49" t="s">
+      <c r="L4" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="M4" s="50"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="49" t="s">
+      <c r="M4" s="48"/>
+      <c r="N4" s="49"/>
+      <c r="O4" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="P4" s="50"/>
-      <c r="Q4" s="51"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="49"/>
     </row>
     <row r="5" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="20">
         <v>111</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="F5" s="29">
+      <c r="F5" s="20">
         <v>45</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="H5" s="29">
+      <c r="H5" s="20">
         <v>10</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="I5" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="J5" s="29" t="s">
+      <c r="J5" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="K5" s="29" t="s">
+      <c r="K5" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="L5" s="49" t="s">
+      <c r="L5" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="M5" s="50"/>
-      <c r="N5" s="51"/>
-      <c r="O5" s="49" t="s">
+      <c r="M5" s="48"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="51"/>
+      <c r="P5" s="48"/>
+      <c r="Q5" s="49"/>
     </row>
     <row r="6" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="F6" s="31">
+      <c r="F6" s="22">
         <v>784</v>
       </c>
-      <c r="G6" s="31" t="s">
+      <c r="G6" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="H6" s="31">
+      <c r="H6" s="22">
         <v>51</v>
       </c>
-      <c r="I6" s="31" t="s">
+      <c r="I6" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="J6" s="31" t="s">
+      <c r="J6" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="K6" s="31" t="s">
+      <c r="K6" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="L6" s="49" t="s">
+      <c r="L6" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="M6" s="50"/>
-      <c r="N6" s="51"/>
-      <c r="O6" s="49" t="s">
+      <c r="M6" s="48"/>
+      <c r="N6" s="49"/>
+      <c r="O6" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="P6" s="50"/>
-      <c r="Q6" s="51"/>
+      <c r="P6" s="48"/>
+      <c r="Q6" s="49"/>
     </row>
     <row r="7" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="25">
         <v>9.9999999999999903E+46</v>
       </c>
-      <c r="E7" s="34" t="s">
+      <c r="E7" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="34">
+      <c r="F7" s="25">
         <v>64152</v>
       </c>
-      <c r="G7" s="34" t="s">
+      <c r="G7" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="H7" s="34">
+      <c r="H7" s="25">
         <v>10</v>
       </c>
-      <c r="I7" s="34" t="s">
+      <c r="I7" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="J7" s="34" t="s">
+      <c r="J7" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="K7" s="34" t="s">
+      <c r="K7" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="L7" s="49" t="s">
+      <c r="L7" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="M7" s="50"/>
-      <c r="N7" s="51"/>
-      <c r="O7" s="49" t="s">
+      <c r="M7" s="48"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="P7" s="50"/>
-      <c r="Q7" s="51"/>
+      <c r="P7" s="48"/>
+      <c r="Q7" s="49"/>
     </row>
     <row r="8" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="25">
         <v>0</v>
       </c>
-      <c r="E8" s="34" t="s">
+      <c r="E8" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="F8" s="34">
+      <c r="F8" s="25">
         <v>145</v>
       </c>
-      <c r="G8" s="34" t="s">
+      <c r="G8" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="H8" s="34">
+      <c r="H8" s="25">
         <v>21</v>
       </c>
-      <c r="I8" s="34" t="s">
+      <c r="I8" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="J8" s="34" t="s">
+      <c r="J8" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="K8" s="34" t="s">
+      <c r="K8" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="L8" s="49" t="s">
+      <c r="L8" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="M8" s="50"/>
-      <c r="N8" s="51"/>
-      <c r="O8" s="49" t="s">
+      <c r="M8" s="48"/>
+      <c r="N8" s="49"/>
+      <c r="O8" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="P8" s="50"/>
-      <c r="Q8" s="51"/>
+      <c r="P8" s="48"/>
+      <c r="Q8" s="49"/>
     </row>
     <row r="9" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="C9" s="58" t="s">
+      <c r="C9" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="D9" s="58">
+      <c r="D9" s="28">
         <v>741541</v>
       </c>
-      <c r="E9" s="58" t="s">
+      <c r="E9" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="F9" s="58">
+      <c r="F9" s="28">
         <v>541</v>
       </c>
-      <c r="G9" s="58" t="s">
+      <c r="G9" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="H9" s="58">
+      <c r="H9" s="28">
         <v>41</v>
       </c>
-      <c r="I9" s="58" t="s">
+      <c r="I9" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="J9" s="58" t="s">
+      <c r="J9" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="K9" s="58" t="s">
+      <c r="K9" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="L9" s="61" t="s">
+      <c r="L9" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="M9" s="62"/>
-      <c r="N9" s="63"/>
-      <c r="O9" s="49" t="s">
+      <c r="M9" s="45"/>
+      <c r="N9" s="46"/>
+      <c r="O9" s="47" t="s">
         <v>117</v>
       </c>
-      <c r="P9" s="50"/>
-      <c r="Q9" s="51"/>
+      <c r="P9" s="48"/>
+      <c r="Q9" s="49"/>
     </row>
     <row r="10" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="59" t="s">
+      <c r="A10" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="C10" s="60" t="s">
+      <c r="C10" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="D10" s="60">
+      <c r="D10" s="30">
         <v>1215</v>
       </c>
-      <c r="E10" s="60" t="s">
+      <c r="E10" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="F10" s="60">
+      <c r="F10" s="30">
         <v>14</v>
       </c>
-      <c r="G10" s="60" t="s">
+      <c r="G10" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="H10" s="60">
+      <c r="H10" s="30">
         <v>100</v>
       </c>
-      <c r="I10" s="60" t="s">
+      <c r="I10" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="J10" s="60" t="s">
+      <c r="J10" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="K10" s="60" t="s">
+      <c r="K10" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="L10" s="61" t="s">
+      <c r="L10" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="M10" s="62"/>
-      <c r="N10" s="63"/>
-      <c r="O10" s="49" t="s">
+      <c r="M10" s="45"/>
+      <c r="N10" s="46"/>
+      <c r="O10" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="P10" s="50"/>
-      <c r="Q10" s="51"/>
+      <c r="P10" s="48"/>
+      <c r="Q10" s="49"/>
     </row>
     <row r="11" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="C11" s="60" t="s">
+      <c r="C11" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="D11" s="60">
+      <c r="D11" s="30">
         <v>424</v>
       </c>
-      <c r="E11" s="60" t="s">
+      <c r="E11" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="F11" s="60">
+      <c r="F11" s="30">
         <v>12541</v>
       </c>
-      <c r="G11" s="60" t="s">
+      <c r="G11" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="H11" s="60">
+      <c r="H11" s="30">
         <v>115</v>
       </c>
-      <c r="I11" s="60" t="s">
+      <c r="I11" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="J11" s="60" t="s">
+      <c r="J11" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="K11" s="60" t="s">
+      <c r="K11" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="L11" s="49" t="s">
+      <c r="L11" s="47" t="s">
         <v>125</v>
       </c>
-      <c r="M11" s="50"/>
-      <c r="N11" s="51"/>
-      <c r="O11" s="49" t="s">
+      <c r="M11" s="48"/>
+      <c r="N11" s="49"/>
+      <c r="O11" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="P11" s="50"/>
-      <c r="Q11" s="51"/>
+      <c r="P11" s="48"/>
+      <c r="Q11" s="49"/>
     </row>
-    <row r="12" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
+      <c r="B12" s="56" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="56" t="s">
+        <v>127</v>
+      </c>
+      <c r="D12" s="56">
+        <v>18748</v>
+      </c>
+      <c r="E12" s="56" t="s">
+        <v>128</v>
+      </c>
+      <c r="F12" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="G12" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="H12" s="56">
+        <v>10</v>
+      </c>
+      <c r="I12" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="J12" s="56" t="s">
+        <v>130</v>
+      </c>
+      <c r="K12" s="56" t="s">
+        <v>103</v>
+      </c>
+      <c r="L12" s="47" t="s">
+        <v>131</v>
+      </c>
+      <c r="M12" s="48"/>
+      <c r="N12" s="49"/>
+      <c r="O12" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="49"/>
     </row>
-    <row r="13" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
+      <c r="B13" s="58" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" s="58" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" s="58">
+        <v>51548</v>
+      </c>
+      <c r="E13" s="58" t="s">
+        <v>133</v>
+      </c>
+      <c r="F13" s="58">
+        <v>9.9999999999999906E+51</v>
+      </c>
+      <c r="G13" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="H13" s="58">
+        <v>21</v>
+      </c>
+      <c r="I13" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="J13" s="58" t="s">
+        <v>134</v>
+      </c>
+      <c r="K13" s="58" t="s">
+        <v>103</v>
+      </c>
+      <c r="L13" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="M13" s="48"/>
+      <c r="N13" s="49"/>
+      <c r="O13" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="P13" s="48"/>
+      <c r="Q13" s="49"/>
     </row>
-    <row r="14" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
+      <c r="B14" s="58" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" s="58" t="s">
+        <v>136</v>
+      </c>
+      <c r="D14" s="58">
+        <v>2115</v>
+      </c>
+      <c r="E14" s="58" t="s">
+        <v>137</v>
+      </c>
+      <c r="F14" s="58">
+        <v>-41</v>
+      </c>
+      <c r="G14" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="H14" s="58">
+        <v>53</v>
+      </c>
+      <c r="I14" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="J14" s="58" t="s">
+        <v>138</v>
+      </c>
+      <c r="K14" s="58" t="s">
+        <v>103</v>
+      </c>
+      <c r="L14" s="44" t="s">
+        <v>93</v>
+      </c>
+      <c r="M14" s="45"/>
+      <c r="N14" s="46"/>
+      <c r="O14" s="47" t="s">
+        <v>139</v>
+      </c>
+      <c r="P14" s="48"/>
+      <c r="Q14" s="49"/>
     </row>
     <row r="15" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="14"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4468,13 +4631,13 @@
     <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="O11:Q11"/>
+  <mergeCells count="26">
+    <mergeCell ref="L12:N12"/>
+    <mergeCell ref="O12:Q12"/>
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="O13:Q13"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="O14:Q14"/>
     <mergeCell ref="L7:N7"/>
     <mergeCell ref="O7:Q7"/>
     <mergeCell ref="L8:N8"/>
@@ -4489,6 +4652,12 @@
     <mergeCell ref="O4:Q4"/>
     <mergeCell ref="L5:N5"/>
     <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="O11:Q11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Se añadio Los casos de Prueba para entradas Stock incorrectas se reporta errores en el CP14
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M3.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00D9B74-5D42-4631-9565-82F86D8FA59D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B8E75D-722C-4C46-B6BE-EACD3FB5D7DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="156">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -721,12 +721,120 @@
   <si>
     <t>Error no se debe Permitir el ingreso de un Stock Negativo</t>
   </si>
+  <si>
+    <t>Registro con Precio Incorrecto</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;, CEV&lt;03&gt; ,CEV&lt;04&gt;,CEV&lt;06&gt;,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;10&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ,CEV&lt;09&gt;,CEV&lt;11&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Portatarjetas de cuero</t>
+  </si>
+  <si>
+    <t>bgrh</t>
+  </si>
+  <si>
+    <t>Pocas Unidades</t>
+  </si>
+  <si>
+    <t>No se permite el ingreso de "bfhfdh" como Precio</t>
+  </si>
+  <si>
+    <t>CP13</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;, CEV&lt;03&gt; ,CEV&lt;04&gt;,CEV&lt;06&gt;,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;11&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">,CEV&lt;09&gt;,CEV&lt;11&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Maletín de cuero</t>
+  </si>
+  <si>
+    <t>Relanzamiento</t>
+  </si>
+  <si>
+    <t>No se permite el ingreso de "99999,,,," como Precio</t>
+  </si>
+  <si>
+    <t>CP14</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;, CEV&lt;03&gt; ,CEV&lt;04&gt;,CEV&lt;06&gt;,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;12&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">,CEV&lt;09&gt;,CEV&lt;11&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Guante de cuero</t>
+  </si>
+  <si>
+    <t>Producto de Diseñador</t>
+  </si>
+  <si>
+    <t>Error no se debe Permitir el ingreso de un Precio Negativo</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -747,27 +855,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <sz val="9"/>
@@ -837,12 +924,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF9FC5E8"/>
-        <bgColor rgb="FF9FC5E8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -877,6 +958,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9FC5E8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -1093,7 +1180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1104,164 +1191,173 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1693,14 +1789,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="43"/>
-      <c r="F3" s="42" t="s">
+      <c r="E3" s="37"/>
+      <c r="F3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="43"/>
+      <c r="G3" s="37"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -1723,310 +1819,310 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="9" t="s">
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="9" t="s">
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="34"/>
-      <c r="C9" s="33" t="s">
+      <c r="B9" s="32"/>
+      <c r="C9" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="12" t="s">
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="8" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="33" t="s">
+      <c r="E11" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="4" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="9" t="s">
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="9" t="s">
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
     </row>
     <row r="15" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
     </row>
     <row r="16" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="12" t="s">
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
     </row>
     <row r="17" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="33" t="s">
+      <c r="C17" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="33" t="s">
+      <c r="E17" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="4" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="9" t="s">
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="G18" s="5" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="9" t="s">
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G19" s="5" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="31" t="s">
+      <c r="E20" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="F20" s="31" t="s">
+      <c r="F20" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="G20" s="31" t="s">
+      <c r="G20" s="34" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="34"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
     </row>
     <row r="22" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="35"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="12" t="s">
+      <c r="B22" s="33"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E22" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
     </row>
     <row r="23" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F23" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="G23" s="7" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="34"/>
-      <c r="C24" s="33" t="s">
+      <c r="B24" s="32"/>
+      <c r="C24" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="31" t="s">
+      <c r="D24" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="E24" s="31" t="s">
+      <c r="E24" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F24" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="G24" s="12" t="s">
+      <c r="G24" s="8" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="12" t="s">
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="G25" s="12" t="s">
+      <c r="G25" s="8" t="s">
         <v>81</v>
       </c>
     </row>
@@ -3009,14 +3105,18 @@
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F16"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="D11:D13"/>
@@ -3031,18 +3131,14 @@
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="E17:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -3054,8 +3150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q991"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13:N13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3081,9 +3177,9 @@
       <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="13"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="9"/>
       <c r="D2" s="52" t="s">
         <v>6</v>
       </c>
@@ -3093,46 +3189,46 @@
       <c r="H2" s="53"/>
       <c r="I2" s="53"/>
       <c r="J2" s="54"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
     </row>
     <row r="3" spans="1:17" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="12" t="s">
         <v>9</v>
       </c>
       <c r="L3" s="52" t="s">
@@ -3147,530 +3243,646 @@
       <c r="Q3" s="54"/>
     </row>
     <row r="4" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="14">
         <v>5</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="14">
         <v>10</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="14">
         <v>50</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="I4" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="K4" s="18" t="s">
+      <c r="K4" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="L4" s="47" t="s">
+      <c r="L4" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="M4" s="48"/>
-      <c r="N4" s="49"/>
-      <c r="O4" s="47" t="s">
+      <c r="M4" s="45"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="P4" s="48"/>
-      <c r="Q4" s="49"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="46"/>
     </row>
     <row r="5" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="16">
         <v>111</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="16">
         <v>45</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="H5" s="20">
+      <c r="H5" s="16">
         <v>10</v>
       </c>
-      <c r="I5" s="20" t="s">
+      <c r="I5" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="J5" s="20" t="s">
+      <c r="J5" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="K5" s="20" t="s">
+      <c r="K5" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="L5" s="47" t="s">
+      <c r="L5" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="M5" s="48"/>
-      <c r="N5" s="49"/>
-      <c r="O5" s="47" t="s">
+      <c r="M5" s="45"/>
+      <c r="N5" s="46"/>
+      <c r="O5" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="P5" s="48"/>
-      <c r="Q5" s="49"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="46"/>
     </row>
     <row r="6" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="18">
         <v>784</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="H6" s="22">
+      <c r="H6" s="18">
         <v>51</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="I6" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="J6" s="22" t="s">
+      <c r="J6" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="K6" s="22" t="s">
+      <c r="K6" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="L6" s="47" t="s">
+      <c r="L6" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="M6" s="48"/>
-      <c r="N6" s="49"/>
-      <c r="O6" s="47" t="s">
+      <c r="M6" s="45"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="P6" s="48"/>
-      <c r="Q6" s="49"/>
+      <c r="P6" s="45"/>
+      <c r="Q6" s="46"/>
     </row>
     <row r="7" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="21">
         <v>9.9999999999999903E+46</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="21">
         <v>64152</v>
       </c>
-      <c r="G7" s="25" t="s">
+      <c r="G7" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="21">
         <v>10</v>
       </c>
-      <c r="I7" s="25" t="s">
+      <c r="I7" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="J7" s="25" t="s">
+      <c r="J7" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="K7" s="25" t="s">
+      <c r="K7" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="L7" s="47" t="s">
+      <c r="L7" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="M7" s="48"/>
-      <c r="N7" s="49"/>
-      <c r="O7" s="47" t="s">
+      <c r="M7" s="45"/>
+      <c r="N7" s="46"/>
+      <c r="O7" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="P7" s="48"/>
-      <c r="Q7" s="49"/>
+      <c r="P7" s="45"/>
+      <c r="Q7" s="46"/>
     </row>
     <row r="8" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="21">
         <v>0</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="21">
         <v>145</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="H8" s="25">
+      <c r="H8" s="21">
         <v>21</v>
       </c>
-      <c r="I8" s="25" t="s">
+      <c r="I8" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="J8" s="25" t="s">
+      <c r="J8" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="K8" s="25" t="s">
+      <c r="K8" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="L8" s="47" t="s">
+      <c r="L8" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="M8" s="48"/>
-      <c r="N8" s="49"/>
-      <c r="O8" s="47" t="s">
+      <c r="M8" s="45"/>
+      <c r="N8" s="46"/>
+      <c r="O8" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="P8" s="48"/>
-      <c r="Q8" s="49"/>
+      <c r="P8" s="45"/>
+      <c r="Q8" s="46"/>
     </row>
     <row r="9" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D9" s="24">
         <v>741541</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="24">
         <v>541</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="H9" s="28">
+      <c r="H9" s="24">
         <v>41</v>
       </c>
-      <c r="I9" s="28" t="s">
+      <c r="I9" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="J9" s="28" t="s">
+      <c r="J9" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="K9" s="28" t="s">
+      <c r="K9" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="L9" s="44" t="s">
+      <c r="L9" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="M9" s="45"/>
-      <c r="N9" s="46"/>
-      <c r="O9" s="47" t="s">
+      <c r="M9" s="48"/>
+      <c r="N9" s="49"/>
+      <c r="O9" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="P9" s="48"/>
-      <c r="Q9" s="49"/>
+      <c r="P9" s="45"/>
+      <c r="Q9" s="46"/>
     </row>
     <row r="10" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="D10" s="30">
+      <c r="D10" s="26">
         <v>1215</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="E10" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F10" s="26">
         <v>14</v>
       </c>
-      <c r="G10" s="30" t="s">
+      <c r="G10" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="H10" s="30">
+      <c r="H10" s="26">
         <v>100</v>
       </c>
-      <c r="I10" s="30" t="s">
+      <c r="I10" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="J10" s="30" t="s">
+      <c r="J10" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="K10" s="30" t="s">
+      <c r="K10" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="L10" s="44" t="s">
+      <c r="L10" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="M10" s="45"/>
-      <c r="N10" s="46"/>
-      <c r="O10" s="47" t="s">
+      <c r="M10" s="48"/>
+      <c r="N10" s="49"/>
+      <c r="O10" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="P10" s="48"/>
-      <c r="Q10" s="49"/>
+      <c r="P10" s="45"/>
+      <c r="Q10" s="46"/>
     </row>
     <row r="11" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="D11" s="30">
+      <c r="D11" s="26">
         <v>424</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="F11" s="30">
+      <c r="F11" s="26">
         <v>12541</v>
       </c>
-      <c r="G11" s="30" t="s">
+      <c r="G11" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="H11" s="30">
+      <c r="H11" s="26">
         <v>115</v>
       </c>
-      <c r="I11" s="30" t="s">
+      <c r="I11" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="J11" s="30" t="s">
+      <c r="J11" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="K11" s="30" t="s">
+      <c r="K11" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="L11" s="47" t="s">
+      <c r="L11" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="M11" s="48"/>
-      <c r="N11" s="49"/>
-      <c r="O11" s="47" t="s">
+      <c r="M11" s="45"/>
+      <c r="N11" s="46"/>
+      <c r="O11" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="P11" s="48"/>
-      <c r="Q11" s="49"/>
+      <c r="P11" s="45"/>
+      <c r="Q11" s="46"/>
     </row>
     <row r="12" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="55" t="s">
+      <c r="A12" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="56" t="s">
+      <c r="B12" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="C12" s="56" t="s">
+      <c r="C12" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="D12" s="56">
+      <c r="D12" s="28">
         <v>18748</v>
       </c>
-      <c r="E12" s="56" t="s">
+      <c r="E12" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="F12" s="56" t="s">
+      <c r="F12" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="G12" s="56" t="s">
+      <c r="G12" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="H12" s="56">
+      <c r="H12" s="28">
         <v>10</v>
       </c>
-      <c r="I12" s="56" t="s">
+      <c r="I12" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="J12" s="56" t="s">
+      <c r="J12" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="K12" s="56" t="s">
+      <c r="K12" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="L12" s="47" t="s">
+      <c r="L12" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="M12" s="48"/>
-      <c r="N12" s="49"/>
-      <c r="O12" s="47" t="s">
+      <c r="M12" s="45"/>
+      <c r="N12" s="46"/>
+      <c r="O12" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="P12" s="48"/>
-      <c r="Q12" s="49"/>
+      <c r="P12" s="45"/>
+      <c r="Q12" s="46"/>
     </row>
     <row r="13" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="57" t="s">
+      <c r="A13" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="C13" s="58" t="s">
+      <c r="C13" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="D13" s="58">
+      <c r="D13" s="30">
         <v>51548</v>
       </c>
-      <c r="E13" s="58" t="s">
+      <c r="E13" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="F13" s="58">
+      <c r="F13" s="30">
         <v>9.9999999999999906E+51</v>
       </c>
-      <c r="G13" s="58" t="s">
+      <c r="G13" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="H13" s="58">
+      <c r="H13" s="30">
         <v>21</v>
       </c>
-      <c r="I13" s="58" t="s">
+      <c r="I13" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="J13" s="58" t="s">
+      <c r="J13" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="K13" s="58" t="s">
+      <c r="K13" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="L13" s="47" t="s">
+      <c r="L13" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="M13" s="48"/>
-      <c r="N13" s="49"/>
-      <c r="O13" s="47" t="s">
+      <c r="M13" s="45"/>
+      <c r="N13" s="46"/>
+      <c r="O13" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="P13" s="48"/>
-      <c r="Q13" s="49"/>
+      <c r="P13" s="45"/>
+      <c r="Q13" s="46"/>
     </row>
     <row r="14" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="57" t="s">
+      <c r="A14" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="58" t="s">
+      <c r="B14" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="C14" s="58" t="s">
+      <c r="C14" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="D14" s="58">
+      <c r="D14" s="30">
         <v>2115</v>
       </c>
-      <c r="E14" s="58" t="s">
+      <c r="E14" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="F14" s="58">
+      <c r="F14" s="30">
         <v>-41</v>
       </c>
-      <c r="G14" s="58" t="s">
+      <c r="G14" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="H14" s="58">
+      <c r="H14" s="30">
         <v>53</v>
       </c>
-      <c r="I14" s="58" t="s">
+      <c r="I14" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="J14" s="58" t="s">
+      <c r="J14" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="K14" s="58" t="s">
+      <c r="K14" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="L14" s="44" t="s">
+      <c r="L14" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="M14" s="45"/>
-      <c r="N14" s="46"/>
-      <c r="O14" s="47" t="s">
+      <c r="M14" s="48"/>
+      <c r="N14" s="49"/>
+      <c r="O14" s="44" t="s">
         <v>139</v>
       </c>
-      <c r="P14" s="48"/>
-      <c r="Q14" s="49"/>
+      <c r="P14" s="45"/>
+      <c r="Q14" s="46"/>
     </row>
-    <row r="15" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="5"/>
+      <c r="B15" s="56" t="s">
+        <v>140</v>
+      </c>
+      <c r="C15" s="56" t="s">
+        <v>141</v>
+      </c>
+      <c r="D15" s="56">
+        <v>1515</v>
+      </c>
+      <c r="E15" s="56" t="s">
+        <v>142</v>
+      </c>
+      <c r="F15" s="56">
+        <v>2054</v>
+      </c>
+      <c r="G15" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="H15" s="56" t="s">
+        <v>143</v>
+      </c>
+      <c r="I15" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="J15" s="56" t="s">
+        <v>144</v>
+      </c>
+      <c r="K15" s="56" t="s">
+        <v>103</v>
+      </c>
+      <c r="L15" s="44" t="s">
+        <v>145</v>
+      </c>
+      <c r="M15" s="45"/>
+      <c r="N15" s="46"/>
+      <c r="O15" s="59"/>
+      <c r="P15" s="60"/>
+      <c r="Q15" s="61"/>
     </row>
-    <row r="16" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="57" t="s">
+        <v>146</v>
+      </c>
+      <c r="B16" s="58" t="s">
+        <v>140</v>
+      </c>
+      <c r="C16" s="58" t="s">
+        <v>147</v>
+      </c>
+      <c r="D16" s="58">
+        <v>151874</v>
+      </c>
+      <c r="E16" s="58" t="s">
+        <v>148</v>
+      </c>
+      <c r="F16" s="58">
+        <v>21</v>
+      </c>
+      <c r="G16" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="H16" s="58">
+        <v>9.99999999999999E+98</v>
+      </c>
+      <c r="I16" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="J16" s="58" t="s">
+        <v>149</v>
+      </c>
+      <c r="K16" s="58" t="s">
+        <v>103</v>
+      </c>
+      <c r="L16" s="44" t="s">
+        <v>150</v>
+      </c>
+      <c r="M16" s="45"/>
+      <c r="N16" s="46"/>
+      <c r="O16" s="59"/>
+      <c r="P16" s="60"/>
+      <c r="Q16" s="61"/>
+    </row>
+    <row r="17" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="57" t="s">
+        <v>151</v>
+      </c>
+      <c r="B17" s="58" t="s">
+        <v>140</v>
+      </c>
+      <c r="C17" s="58" t="s">
+        <v>152</v>
+      </c>
+      <c r="D17" s="58">
+        <v>584</v>
+      </c>
+      <c r="E17" s="58" t="s">
+        <v>153</v>
+      </c>
+      <c r="F17" s="58">
+        <v>1</v>
+      </c>
+      <c r="G17" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17" s="58">
+        <v>-500</v>
+      </c>
+      <c r="I17" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="J17" s="58" t="s">
+        <v>154</v>
+      </c>
+      <c r="K17" s="58" t="s">
+        <v>103</v>
+      </c>
+      <c r="L17" s="47" t="s">
+        <v>93</v>
+      </c>
+      <c r="M17" s="48"/>
+      <c r="N17" s="49"/>
+      <c r="O17" s="44" t="s">
+        <v>155</v>
+      </c>
+      <c r="P17" s="45"/>
+      <c r="Q17" s="46"/>
+    </row>
+    <row r="18" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4631,13 +4843,19 @@
     <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="O12:Q12"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="O13:Q13"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="O14:Q14"/>
+  <mergeCells count="32">
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="O15:Q15"/>
+    <mergeCell ref="L16:N16"/>
+    <mergeCell ref="O16:Q16"/>
+    <mergeCell ref="L17:N17"/>
+    <mergeCell ref="O17:Q17"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="O11:Q11"/>
     <mergeCell ref="L7:N7"/>
     <mergeCell ref="O7:Q7"/>
     <mergeCell ref="L8:N8"/>
@@ -4652,12 +4870,12 @@
     <mergeCell ref="O4:Q4"/>
     <mergeCell ref="L5:N5"/>
     <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="O11:Q11"/>
+    <mergeCell ref="L12:N12"/>
+    <mergeCell ref="O12:Q12"/>
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="O13:Q13"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="O14:Q14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Se añadio Los casos de Prueba para entradas Fotos incorrectas se reporta errores en el CP15
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M3.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B8E75D-722C-4C46-B6BE-EACD3FB5D7DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428A7C5E-7A80-4CA4-ABCB-9CD04395CCA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="164">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -828,6 +828,50 @@
   </si>
   <si>
     <t>Error no se debe Permitir el ingreso de un Precio Negativo</t>
+  </si>
+  <si>
+    <t>CP15</t>
+  </si>
+  <si>
+    <t>Registro con Fotos Incorrecto</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;,CEV&lt;02&gt;,CEV&lt;04&gt;,CEV&lt;05&gt;,CEV&lt;07&gt;,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;13&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ,CEV&lt;10&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Libreta de cuero</t>
+  </si>
+  <si>
+    <t>Libretas</t>
+  </si>
+  <si>
+    <t>Documento PDF</t>
+  </si>
+  <si>
+    <t>Nuevo Lanzamiento</t>
+  </si>
+  <si>
+    <t>Error no se debe Permitir el ingreso de un archivo que no esté en formato de imágen como Fotos</t>
   </si>
 </sst>
 </file>
@@ -909,7 +953,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -964,6 +1008,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD5A6BD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -1180,7 +1230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1272,6 +1322,24 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1281,34 +1349,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1317,6 +1379,15 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1338,26 +1409,11 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1789,14 +1845,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="36" t="s">
+      <c r="E3" s="47"/>
+      <c r="F3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="37"/>
+      <c r="G3" s="47"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -1819,16 +1875,16 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="37" t="s">
         <v>25</v>
       </c>
       <c r="F5" s="4" t="s">
@@ -1839,10 +1895,10 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
       <c r="F6" s="5" t="s">
         <v>28</v>
       </c>
@@ -1851,10 +1907,10 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
       <c r="F7" s="5" t="s">
         <v>30</v>
       </c>
@@ -1863,7 +1919,7 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="37" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -1883,14 +1939,14 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="32"/>
-      <c r="C9" s="31" t="s">
+      <c r="B9" s="38"/>
+      <c r="C9" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="D9" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="E9" s="35" t="s">
         <v>40</v>
       </c>
       <c r="F9" s="8" t="s">
@@ -1901,10 +1957,10 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
       <c r="F10" s="8" t="s">
         <v>43</v>
       </c>
@@ -1913,16 +1969,16 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="37" t="s">
         <v>47</v>
       </c>
       <c r="F11" s="4" t="s">
@@ -1933,10 +1989,10 @@
       </c>
     </row>
     <row r="12" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
       <c r="F12" s="5" t="s">
         <v>50</v>
       </c>
@@ -1945,10 +2001,10 @@
       </c>
     </row>
     <row r="13" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
       <c r="F13" s="5" t="s">
         <v>52</v>
       </c>
@@ -1957,52 +2013,52 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="34" t="s">
+      <c r="D14" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="34" t="s">
+      <c r="E14" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
     </row>
     <row r="15" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
     </row>
     <row r="16" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
       <c r="D16" s="8" t="s">
         <v>58</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
     </row>
     <row r="17" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="E17" s="37" t="s">
         <v>62</v>
       </c>
       <c r="F17" s="4" t="s">
@@ -2013,10 +2069,10 @@
       </c>
     </row>
     <row r="18" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
       <c r="F18" s="5" t="s">
         <v>65</v>
       </c>
@@ -2025,10 +2081,10 @@
       </c>
     </row>
     <row r="19" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
       <c r="F19" s="5" t="s">
         <v>52</v>
       </c>
@@ -2037,36 +2093,36 @@
       </c>
     </row>
     <row r="20" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="41" t="s">
+      <c r="C20" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="D20" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="34" t="s">
+      <c r="E20" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="F20" s="34" t="s">
+      <c r="F20" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="G20" s="34" t="s">
+      <c r="G20" s="35" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="32"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
     </row>
     <row r="22" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="33"/>
-      <c r="C22" s="43"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="42"/>
       <c r="D22" s="8" t="s">
         <v>73</v>
       </c>
@@ -2077,7 +2133,7 @@
       <c r="G22" s="9"/>
     </row>
     <row r="23" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="37" t="s">
         <v>82</v>
       </c>
       <c r="C23" s="6" t="s">
@@ -2097,14 +2153,14 @@
       </c>
     </row>
     <row r="24" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="32"/>
-      <c r="C24" s="31" t="s">
+      <c r="B24" s="38"/>
+      <c r="C24" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="34" t="s">
+      <c r="D24" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="E24" s="34" t="s">
+      <c r="E24" s="35" t="s">
         <v>78</v>
       </c>
       <c r="F24" s="8" t="s">
@@ -2115,10 +2171,10 @@
       </c>
     </row>
     <row r="25" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
       <c r="F25" s="8" t="s">
         <v>80</v>
       </c>
@@ -3105,18 +3161,14 @@
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="E17:E19"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="D11:D13"/>
@@ -3131,14 +3183,18 @@
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -3150,8 +3206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q991"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3170,25 +3226,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="9"/>
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="54"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="61"/>
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
       <c r="M2" s="10"/>
@@ -3231,16 +3287,16 @@
       <c r="K3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="52" t="s">
+      <c r="L3" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="53"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="52" t="s">
+      <c r="M3" s="60"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="P3" s="53"/>
-      <c r="Q3" s="54"/>
+      <c r="P3" s="60"/>
+      <c r="Q3" s="61"/>
     </row>
     <row r="4" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -3276,16 +3332,16 @@
       <c r="K4" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="L4" s="44" t="s">
+      <c r="L4" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="M4" s="45"/>
-      <c r="N4" s="46"/>
-      <c r="O4" s="44" t="s">
+      <c r="M4" s="49"/>
+      <c r="N4" s="50"/>
+      <c r="O4" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="P4" s="45"/>
-      <c r="Q4" s="46"/>
+      <c r="P4" s="49"/>
+      <c r="Q4" s="50"/>
     </row>
     <row r="5" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
@@ -3321,16 +3377,16 @@
       <c r="K5" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="L5" s="44" t="s">
+      <c r="L5" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="M5" s="45"/>
-      <c r="N5" s="46"/>
-      <c r="O5" s="44" t="s">
+      <c r="M5" s="49"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="46"/>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="50"/>
     </row>
     <row r="6" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
@@ -3366,16 +3422,16 @@
       <c r="K6" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="L6" s="44" t="s">
+      <c r="L6" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="M6" s="45"/>
-      <c r="N6" s="46"/>
-      <c r="O6" s="44" t="s">
+      <c r="M6" s="49"/>
+      <c r="N6" s="50"/>
+      <c r="O6" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="P6" s="45"/>
-      <c r="Q6" s="46"/>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="50"/>
     </row>
     <row r="7" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
@@ -3411,16 +3467,16 @@
       <c r="K7" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="L7" s="44" t="s">
+      <c r="L7" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="M7" s="45"/>
-      <c r="N7" s="46"/>
-      <c r="O7" s="44" t="s">
+      <c r="M7" s="49"/>
+      <c r="N7" s="50"/>
+      <c r="O7" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="P7" s="45"/>
-      <c r="Q7" s="46"/>
+      <c r="P7" s="49"/>
+      <c r="Q7" s="50"/>
     </row>
     <row r="8" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
@@ -3456,16 +3512,16 @@
       <c r="K8" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="L8" s="44" t="s">
+      <c r="L8" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="M8" s="45"/>
-      <c r="N8" s="46"/>
-      <c r="O8" s="44" t="s">
+      <c r="M8" s="49"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="P8" s="45"/>
-      <c r="Q8" s="46"/>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="50"/>
     </row>
     <row r="9" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
@@ -3501,16 +3557,16 @@
       <c r="K9" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="L9" s="47" t="s">
+      <c r="L9" s="54" t="s">
         <v>93</v>
       </c>
-      <c r="M9" s="48"/>
-      <c r="N9" s="49"/>
-      <c r="O9" s="44" t="s">
+      <c r="M9" s="55"/>
+      <c r="N9" s="56"/>
+      <c r="O9" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="P9" s="45"/>
-      <c r="Q9" s="46"/>
+      <c r="P9" s="49"/>
+      <c r="Q9" s="50"/>
     </row>
     <row r="10" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
@@ -3546,16 +3602,16 @@
       <c r="K10" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="L10" s="47" t="s">
+      <c r="L10" s="54" t="s">
         <v>93</v>
       </c>
-      <c r="M10" s="48"/>
-      <c r="N10" s="49"/>
-      <c r="O10" s="44" t="s">
+      <c r="M10" s="55"/>
+      <c r="N10" s="56"/>
+      <c r="O10" s="48" t="s">
         <v>121</v>
       </c>
-      <c r="P10" s="45"/>
-      <c r="Q10" s="46"/>
+      <c r="P10" s="49"/>
+      <c r="Q10" s="50"/>
     </row>
     <row r="11" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
@@ -3591,16 +3647,16 @@
       <c r="K11" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="L11" s="44" t="s">
+      <c r="L11" s="48" t="s">
         <v>125</v>
       </c>
-      <c r="M11" s="45"/>
-      <c r="N11" s="46"/>
-      <c r="O11" s="44" t="s">
+      <c r="M11" s="49"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="P11" s="45"/>
-      <c r="Q11" s="46"/>
+      <c r="P11" s="49"/>
+      <c r="Q11" s="50"/>
     </row>
     <row r="12" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
@@ -3636,16 +3692,16 @@
       <c r="K12" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="L12" s="44" t="s">
+      <c r="L12" s="48" t="s">
         <v>131</v>
       </c>
-      <c r="M12" s="45"/>
-      <c r="N12" s="46"/>
-      <c r="O12" s="44" t="s">
+      <c r="M12" s="49"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="P12" s="45"/>
-      <c r="Q12" s="46"/>
+      <c r="P12" s="49"/>
+      <c r="Q12" s="50"/>
     </row>
     <row r="13" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
@@ -3681,16 +3737,16 @@
       <c r="K13" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="L13" s="44" t="s">
+      <c r="L13" s="48" t="s">
         <v>135</v>
       </c>
-      <c r="M13" s="45"/>
-      <c r="N13" s="46"/>
-      <c r="O13" s="44" t="s">
+      <c r="M13" s="49"/>
+      <c r="N13" s="50"/>
+      <c r="O13" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="P13" s="45"/>
-      <c r="Q13" s="46"/>
+      <c r="P13" s="49"/>
+      <c r="Q13" s="50"/>
     </row>
     <row r="14" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
@@ -3726,149 +3782,193 @@
       <c r="K14" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="L14" s="47" t="s">
+      <c r="L14" s="54" t="s">
         <v>93</v>
       </c>
-      <c r="M14" s="48"/>
-      <c r="N14" s="49"/>
-      <c r="O14" s="44" t="s">
+      <c r="M14" s="55"/>
+      <c r="N14" s="56"/>
+      <c r="O14" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="P14" s="45"/>
-      <c r="Q14" s="46"/>
+      <c r="P14" s="49"/>
+      <c r="Q14" s="50"/>
     </row>
     <row r="15" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="55" t="s">
+      <c r="A15" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="C15" s="56" t="s">
+      <c r="C15" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="D15" s="56">
+      <c r="D15" s="32">
         <v>1515</v>
       </c>
-      <c r="E15" s="56" t="s">
+      <c r="E15" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="F15" s="56">
+      <c r="F15" s="32">
         <v>2054</v>
       </c>
-      <c r="G15" s="56" t="s">
+      <c r="G15" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="H15" s="56" t="s">
+      <c r="H15" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="I15" s="56" t="s">
+      <c r="I15" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="J15" s="56" t="s">
+      <c r="J15" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="K15" s="56" t="s">
+      <c r="K15" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="L15" s="44" t="s">
+      <c r="L15" s="48" t="s">
         <v>145</v>
       </c>
-      <c r="M15" s="45"/>
-      <c r="N15" s="46"/>
-      <c r="O15" s="59"/>
-      <c r="P15" s="60"/>
-      <c r="Q15" s="61"/>
+      <c r="M15" s="49"/>
+      <c r="N15" s="50"/>
+      <c r="O15" s="51"/>
+      <c r="P15" s="52"/>
+      <c r="Q15" s="53"/>
     </row>
     <row r="16" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="57" t="s">
+      <c r="A16" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="C16" s="58" t="s">
+      <c r="C16" s="34" t="s">
         <v>147</v>
       </c>
-      <c r="D16" s="58">
+      <c r="D16" s="34">
         <v>151874</v>
       </c>
-      <c r="E16" s="58" t="s">
+      <c r="E16" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="F16" s="58">
+      <c r="F16" s="34">
         <v>21</v>
       </c>
-      <c r="G16" s="58" t="s">
+      <c r="G16" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="H16" s="58">
+      <c r="H16" s="34">
         <v>9.99999999999999E+98</v>
       </c>
-      <c r="I16" s="58" t="s">
+      <c r="I16" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="J16" s="58" t="s">
+      <c r="J16" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="K16" s="58" t="s">
+      <c r="K16" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="L16" s="44" t="s">
+      <c r="L16" s="48" t="s">
         <v>150</v>
       </c>
-      <c r="M16" s="45"/>
-      <c r="N16" s="46"/>
-      <c r="O16" s="59"/>
-      <c r="P16" s="60"/>
-      <c r="Q16" s="61"/>
+      <c r="M16" s="49"/>
+      <c r="N16" s="50"/>
+      <c r="O16" s="51"/>
+      <c r="P16" s="52"/>
+      <c r="Q16" s="53"/>
     </row>
     <row r="17" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="C17" s="58" t="s">
+      <c r="C17" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="D17" s="58">
+      <c r="D17" s="34">
         <v>584</v>
       </c>
-      <c r="E17" s="58" t="s">
+      <c r="E17" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="F17" s="58">
+      <c r="F17" s="34">
         <v>1</v>
       </c>
-      <c r="G17" s="58" t="s">
+      <c r="G17" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="H17" s="58">
+      <c r="H17" s="34">
         <v>-500</v>
       </c>
-      <c r="I17" s="58" t="s">
+      <c r="I17" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="J17" s="58" t="s">
+      <c r="J17" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="K17" s="58" t="s">
+      <c r="K17" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="L17" s="47" t="s">
+      <c r="L17" s="54" t="s">
         <v>93</v>
       </c>
-      <c r="M17" s="48"/>
-      <c r="N17" s="49"/>
-      <c r="O17" s="44" t="s">
+      <c r="M17" s="55"/>
+      <c r="N17" s="56"/>
+      <c r="O17" s="48" t="s">
         <v>155</v>
       </c>
-      <c r="P17" s="45"/>
-      <c r="Q17" s="46"/>
+      <c r="P17" s="49"/>
+      <c r="Q17" s="50"/>
     </row>
-    <row r="18" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="1:17" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="62" t="s">
+        <v>156</v>
+      </c>
+      <c r="B18" s="63" t="s">
+        <v>157</v>
+      </c>
+      <c r="C18" s="63" t="s">
+        <v>158</v>
+      </c>
+      <c r="D18" s="63">
+        <v>121515</v>
+      </c>
+      <c r="E18" s="63" t="s">
+        <v>159</v>
+      </c>
+      <c r="F18" s="63">
+        <v>5</v>
+      </c>
+      <c r="G18" s="63" t="s">
+        <v>160</v>
+      </c>
+      <c r="H18" s="63">
+        <v>501</v>
+      </c>
+      <c r="I18" s="63" t="s">
+        <v>161</v>
+      </c>
+      <c r="J18" s="63" t="s">
+        <v>162</v>
+      </c>
+      <c r="K18" s="63" t="s">
+        <v>103</v>
+      </c>
+      <c r="L18" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="M18" s="55"/>
+      <c r="N18" s="56"/>
+      <c r="O18" s="48" t="s">
+        <v>163</v>
+      </c>
+      <c r="P18" s="49"/>
+      <c r="Q18" s="50"/>
+    </row>
     <row r="19" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="21" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4843,19 +4943,15 @@
     <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="O15:Q15"/>
-    <mergeCell ref="L16:N16"/>
-    <mergeCell ref="O16:Q16"/>
-    <mergeCell ref="L17:N17"/>
-    <mergeCell ref="O17:Q17"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="O11:Q11"/>
+  <mergeCells count="34">
+    <mergeCell ref="L18:N18"/>
+    <mergeCell ref="O18:Q18"/>
+    <mergeCell ref="L12:N12"/>
+    <mergeCell ref="O12:Q12"/>
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="O13:Q13"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="O14:Q14"/>
     <mergeCell ref="L7:N7"/>
     <mergeCell ref="O7:Q7"/>
     <mergeCell ref="L8:N8"/>
@@ -4870,12 +4966,18 @@
     <mergeCell ref="O4:Q4"/>
     <mergeCell ref="L5:N5"/>
     <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="O12:Q12"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="O13:Q13"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="O14:Q14"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="O11:Q11"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="O15:Q15"/>
+    <mergeCell ref="L16:N16"/>
+    <mergeCell ref="O16:Q16"/>
+    <mergeCell ref="L17:N17"/>
+    <mergeCell ref="O17:Q17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Se añadio Los casos de Prueba para entradas Observaciones incorrectas se reporta errores en el CP16 y CP17
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M3.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Desktop\GIthub\Softgenix-Peru\2-Desarrollo\SCIP\pruebas-calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428A7C5E-7A80-4CA4-ABCB-9CD04395CCA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFB0725-9F81-47F9-B4EE-8F10A42B2A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="181">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -872,6 +872,109 @@
   </si>
   <si>
     <t>Error no se debe Permitir el ingreso de un archivo que no esté en formato de imágen como Fotos</t>
+  </si>
+  <si>
+    <t>CP16</t>
+  </si>
+  <si>
+    <t>Registro con Observaciones Incorrecto</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;,CEV&lt;02&gt;,CEV&lt;04&gt;,CEV&lt;05&gt;,CEV&lt;07&gt;,CEV&lt;08&gt;,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;14&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Sombrero de cuero
+</t>
+  </si>
+  <si>
+    <t>Sombreros</t>
+  </si>
+  <si>
+    <t>*//%</t>
+  </si>
+  <si>
+    <t>Error no se deben admitir carácteres no alfanuméricos como Observaciones</t>
+  </si>
+  <si>
+    <t>CP17</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;,CEV&lt;02&gt;,CEV&lt;04&gt;,CEV&lt;05&gt;,CEV&lt;07&gt;,CEV&lt;08&gt;,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">CENV&lt;15&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Bota de cuero</t>
+  </si>
+  <si>
+    <t>Botas</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>Error no se deben admitir Observaciones de una letra</t>
+  </si>
+  <si>
+    <t>CP18</t>
+  </si>
+  <si>
+    <r>
+      <t>CEV&lt;01&gt;,CEV&lt;02&gt;,CEV&lt;04&gt;,CEV&lt;05&gt;,CEV&lt;07&gt;,CEV&lt;08&gt;,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CENV&lt;16&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>safdffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffff</t>
+  </si>
+  <si>
+    <t>No se permite el ingreso de "safdfffffffffffffffffffffff,,,,," como Observaciones</t>
   </si>
 </sst>
 </file>
@@ -953,7 +1056,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1014,6 +1117,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCE5CD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -1230,7 +1339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1334,20 +1443,39 @@
     <xf numFmtId="0" fontId="9" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1358,19 +1486,15 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1378,24 +1502,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1409,10 +1515,25 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1826,7 +1947,7 @@
   <dimension ref="B1:G1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1845,14 +1966,14 @@
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="47"/>
-      <c r="F3" s="46" t="s">
+      <c r="E3" s="43"/>
+      <c r="F3" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="47"/>
+      <c r="G3" s="43"/>
     </row>
     <row r="4" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -1943,10 +2064,10 @@
       <c r="C9" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="40" t="s">
         <v>40</v>
       </c>
       <c r="F9" s="8" t="s">
@@ -1959,8 +2080,8 @@
     <row r="10" spans="2:7" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="39"/>
       <c r="C10" s="39"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
       <c r="F10" s="8" t="s">
         <v>43</v>
       </c>
@@ -2019,22 +2140,22 @@
       <c r="C14" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="35" t="s">
+      <c r="D14" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="35" t="s">
+      <c r="E14" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
     </row>
     <row r="15" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="38"/>
       <c r="C15" s="38"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
     </row>
     <row r="16" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="39"/>
@@ -2045,8 +2166,8 @@
       <c r="E16" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
     </row>
     <row r="17" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="37" t="s">
@@ -2096,33 +2217,33 @@
       <c r="B20" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="35" t="s">
+      <c r="D20" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="35" t="s">
+      <c r="E20" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="F20" s="35" t="s">
+      <c r="F20" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="G20" s="35" t="s">
+      <c r="G20" s="40" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="38"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
     </row>
     <row r="22" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="39"/>
-      <c r="C22" s="42"/>
+      <c r="C22" s="49"/>
       <c r="D22" s="8" t="s">
         <v>73</v>
       </c>
@@ -2157,10 +2278,10 @@
       <c r="C24" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="35" t="s">
+      <c r="D24" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="E24" s="35" t="s">
+      <c r="E24" s="40" t="s">
         <v>78</v>
       </c>
       <c r="F24" s="8" t="s">
@@ -2173,8 +2294,8 @@
     <row r="25" spans="2:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="39"/>
       <c r="C25" s="39"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
       <c r="F25" s="8" t="s">
         <v>80</v>
       </c>
@@ -3161,14 +3282,18 @@
     <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F16"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="D11:D13"/>
@@ -3183,18 +3308,14 @@
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="E17:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -3206,8 +3327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q991"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3226,25 +3347,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="9"/>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="61"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="60"/>
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
       <c r="M2" s="10"/>
@@ -3287,16 +3408,16 @@
       <c r="K3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="59" t="s">
+      <c r="L3" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="60"/>
-      <c r="N3" s="61"/>
-      <c r="O3" s="59" t="s">
+      <c r="M3" s="59"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="61"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="60"/>
     </row>
     <row r="4" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -3332,16 +3453,16 @@
       <c r="K4" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="L4" s="48" t="s">
+      <c r="L4" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="M4" s="49"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="48" t="s">
+      <c r="M4" s="54"/>
+      <c r="N4" s="55"/>
+      <c r="O4" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="P4" s="49"/>
-      <c r="Q4" s="50"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="55"/>
     </row>
     <row r="5" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
@@ -3377,16 +3498,16 @@
       <c r="K5" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="L5" s="48" t="s">
+      <c r="L5" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="M5" s="49"/>
-      <c r="N5" s="50"/>
-      <c r="O5" s="48" t="s">
+      <c r="M5" s="54"/>
+      <c r="N5" s="55"/>
+      <c r="O5" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="P5" s="49"/>
-      <c r="Q5" s="50"/>
+      <c r="P5" s="54"/>
+      <c r="Q5" s="55"/>
     </row>
     <row r="6" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
@@ -3422,16 +3543,16 @@
       <c r="K6" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="L6" s="48" t="s">
+      <c r="L6" s="53" t="s">
         <v>104</v>
       </c>
-      <c r="M6" s="49"/>
-      <c r="N6" s="50"/>
-      <c r="O6" s="48" t="s">
+      <c r="M6" s="54"/>
+      <c r="N6" s="55"/>
+      <c r="O6" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="P6" s="49"/>
-      <c r="Q6" s="50"/>
+      <c r="P6" s="54"/>
+      <c r="Q6" s="55"/>
     </row>
     <row r="7" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
@@ -3467,16 +3588,16 @@
       <c r="K7" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="L7" s="48" t="s">
+      <c r="L7" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="M7" s="49"/>
-      <c r="N7" s="50"/>
-      <c r="O7" s="48" t="s">
+      <c r="M7" s="54"/>
+      <c r="N7" s="55"/>
+      <c r="O7" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="P7" s="49"/>
-      <c r="Q7" s="50"/>
+      <c r="P7" s="54"/>
+      <c r="Q7" s="55"/>
     </row>
     <row r="8" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
@@ -3512,16 +3633,16 @@
       <c r="K8" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="L8" s="48" t="s">
+      <c r="L8" s="53" t="s">
         <v>112</v>
       </c>
-      <c r="M8" s="49"/>
-      <c r="N8" s="50"/>
-      <c r="O8" s="48" t="s">
+      <c r="M8" s="54"/>
+      <c r="N8" s="55"/>
+      <c r="O8" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="P8" s="49"/>
-      <c r="Q8" s="50"/>
+      <c r="P8" s="54"/>
+      <c r="Q8" s="55"/>
     </row>
     <row r="9" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
@@ -3557,16 +3678,16 @@
       <c r="K9" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="L9" s="54" t="s">
+      <c r="L9" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="M9" s="55"/>
-      <c r="N9" s="56"/>
-      <c r="O9" s="48" t="s">
+      <c r="M9" s="51"/>
+      <c r="N9" s="52"/>
+      <c r="O9" s="53" t="s">
         <v>117</v>
       </c>
-      <c r="P9" s="49"/>
-      <c r="Q9" s="50"/>
+      <c r="P9" s="54"/>
+      <c r="Q9" s="55"/>
     </row>
     <row r="10" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
@@ -3602,16 +3723,16 @@
       <c r="K10" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="L10" s="54" t="s">
+      <c r="L10" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="M10" s="55"/>
-      <c r="N10" s="56"/>
-      <c r="O10" s="48" t="s">
+      <c r="M10" s="51"/>
+      <c r="N10" s="52"/>
+      <c r="O10" s="53" t="s">
         <v>121</v>
       </c>
-      <c r="P10" s="49"/>
-      <c r="Q10" s="50"/>
+      <c r="P10" s="54"/>
+      <c r="Q10" s="55"/>
     </row>
     <row r="11" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
@@ -3647,16 +3768,16 @@
       <c r="K11" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="L11" s="48" t="s">
+      <c r="L11" s="53" t="s">
         <v>125</v>
       </c>
-      <c r="M11" s="49"/>
-      <c r="N11" s="50"/>
-      <c r="O11" s="48" t="s">
+      <c r="M11" s="54"/>
+      <c r="N11" s="55"/>
+      <c r="O11" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="P11" s="49"/>
-      <c r="Q11" s="50"/>
+      <c r="P11" s="54"/>
+      <c r="Q11" s="55"/>
     </row>
     <row r="12" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
@@ -3692,16 +3813,16 @@
       <c r="K12" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="L12" s="48" t="s">
+      <c r="L12" s="53" t="s">
         <v>131</v>
       </c>
-      <c r="M12" s="49"/>
-      <c r="N12" s="50"/>
-      <c r="O12" s="48" t="s">
+      <c r="M12" s="54"/>
+      <c r="N12" s="55"/>
+      <c r="O12" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="P12" s="49"/>
-      <c r="Q12" s="50"/>
+      <c r="P12" s="54"/>
+      <c r="Q12" s="55"/>
     </row>
     <row r="13" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
@@ -3737,16 +3858,16 @@
       <c r="K13" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="L13" s="48" t="s">
+      <c r="L13" s="53" t="s">
         <v>135</v>
       </c>
-      <c r="M13" s="49"/>
-      <c r="N13" s="50"/>
-      <c r="O13" s="48" t="s">
+      <c r="M13" s="54"/>
+      <c r="N13" s="55"/>
+      <c r="O13" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="P13" s="49"/>
-      <c r="Q13" s="50"/>
+      <c r="P13" s="54"/>
+      <c r="Q13" s="55"/>
     </row>
     <row r="14" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
@@ -3782,16 +3903,16 @@
       <c r="K14" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="L14" s="54" t="s">
+      <c r="L14" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="M14" s="55"/>
-      <c r="N14" s="56"/>
-      <c r="O14" s="48" t="s">
+      <c r="M14" s="51"/>
+      <c r="N14" s="52"/>
+      <c r="O14" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="P14" s="49"/>
-      <c r="Q14" s="50"/>
+      <c r="P14" s="54"/>
+      <c r="Q14" s="55"/>
     </row>
     <row r="15" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
@@ -3827,14 +3948,14 @@
       <c r="K15" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="L15" s="48" t="s">
+      <c r="L15" s="53" t="s">
         <v>145</v>
       </c>
-      <c r="M15" s="49"/>
-      <c r="N15" s="50"/>
-      <c r="O15" s="51"/>
-      <c r="P15" s="52"/>
-      <c r="Q15" s="53"/>
+      <c r="M15" s="54"/>
+      <c r="N15" s="55"/>
+      <c r="O15" s="61"/>
+      <c r="P15" s="62"/>
+      <c r="Q15" s="63"/>
     </row>
     <row r="16" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
@@ -3870,14 +3991,14 @@
       <c r="K16" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="L16" s="48" t="s">
+      <c r="L16" s="53" t="s">
         <v>150</v>
       </c>
-      <c r="M16" s="49"/>
-      <c r="N16" s="50"/>
-      <c r="O16" s="51"/>
-      <c r="P16" s="52"/>
-      <c r="Q16" s="53"/>
+      <c r="M16" s="54"/>
+      <c r="N16" s="55"/>
+      <c r="O16" s="61"/>
+      <c r="P16" s="62"/>
+      <c r="Q16" s="63"/>
     </row>
     <row r="17" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
@@ -3913,65 +4034,197 @@
       <c r="K17" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="L17" s="54" t="s">
+      <c r="L17" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="M17" s="55"/>
-      <c r="N17" s="56"/>
-      <c r="O17" s="48" t="s">
+      <c r="M17" s="51"/>
+      <c r="N17" s="52"/>
+      <c r="O17" s="53" t="s">
         <v>155</v>
       </c>
-      <c r="P17" s="49"/>
-      <c r="Q17" s="50"/>
+      <c r="P17" s="54"/>
+      <c r="Q17" s="55"/>
     </row>
     <row r="18" spans="1:17" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="62" t="s">
+      <c r="A18" s="35" t="s">
         <v>156</v>
       </c>
-      <c r="B18" s="63" t="s">
+      <c r="B18" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="C18" s="63" t="s">
+      <c r="C18" s="36" t="s">
         <v>158</v>
       </c>
-      <c r="D18" s="63">
+      <c r="D18" s="36">
         <v>121515</v>
       </c>
-      <c r="E18" s="63" t="s">
+      <c r="E18" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="F18" s="63">
+      <c r="F18" s="36">
         <v>5</v>
       </c>
-      <c r="G18" s="63" t="s">
+      <c r="G18" s="36" t="s">
         <v>160</v>
       </c>
-      <c r="H18" s="63">
+      <c r="H18" s="36">
         <v>501</v>
       </c>
-      <c r="I18" s="63" t="s">
+      <c r="I18" s="36" t="s">
         <v>161</v>
       </c>
-      <c r="J18" s="63" t="s">
+      <c r="J18" s="36" t="s">
         <v>162</v>
       </c>
-      <c r="K18" s="63" t="s">
+      <c r="K18" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="L18" s="54" t="s">
+      <c r="L18" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="M18" s="55"/>
-      <c r="N18" s="56"/>
-      <c r="O18" s="48" t="s">
+      <c r="M18" s="51"/>
+      <c r="N18" s="52"/>
+      <c r="O18" s="53" t="s">
         <v>163</v>
       </c>
-      <c r="P18" s="49"/>
-      <c r="Q18" s="50"/>
+      <c r="P18" s="54"/>
+      <c r="Q18" s="55"/>
     </row>
-    <row r="19" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:17" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="64" t="s">
+        <v>164</v>
+      </c>
+      <c r="B19" s="65" t="s">
+        <v>165</v>
+      </c>
+      <c r="C19" s="65" t="s">
+        <v>166</v>
+      </c>
+      <c r="D19" s="65">
+        <v>515</v>
+      </c>
+      <c r="E19" s="65" t="s">
+        <v>167</v>
+      </c>
+      <c r="F19" s="65">
+        <v>0</v>
+      </c>
+      <c r="G19" s="65" t="s">
+        <v>168</v>
+      </c>
+      <c r="H19" s="65">
+        <v>10</v>
+      </c>
+      <c r="I19" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="J19" s="65" t="s">
+        <v>169</v>
+      </c>
+      <c r="K19" s="65" t="s">
+        <v>103</v>
+      </c>
+      <c r="L19" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="M19" s="51"/>
+      <c r="N19" s="52"/>
+      <c r="O19" s="53" t="s">
+        <v>170</v>
+      </c>
+      <c r="P19" s="54"/>
+      <c r="Q19" s="55"/>
+    </row>
+    <row r="20" spans="1:17" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="66" t="s">
+        <v>171</v>
+      </c>
+      <c r="B20" s="67" t="s">
+        <v>165</v>
+      </c>
+      <c r="C20" s="67" t="s">
+        <v>172</v>
+      </c>
+      <c r="D20" s="67">
+        <v>4212</v>
+      </c>
+      <c r="E20" s="67" t="s">
+        <v>173</v>
+      </c>
+      <c r="F20" s="67">
+        <v>54</v>
+      </c>
+      <c r="G20" s="67" t="s">
+        <v>174</v>
+      </c>
+      <c r="H20" s="67">
+        <v>15</v>
+      </c>
+      <c r="I20" s="67" t="s">
+        <v>90</v>
+      </c>
+      <c r="J20" s="67" t="s">
+        <v>175</v>
+      </c>
+      <c r="K20" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="L20" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="M20" s="51"/>
+      <c r="N20" s="52"/>
+      <c r="O20" s="53" t="s">
+        <v>176</v>
+      </c>
+      <c r="P20" s="54"/>
+      <c r="Q20" s="55"/>
+    </row>
+    <row r="21" spans="1:17" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="66" t="s">
+        <v>177</v>
+      </c>
+      <c r="B21" s="67" t="s">
+        <v>165</v>
+      </c>
+      <c r="C21" s="67" t="s">
+        <v>178</v>
+      </c>
+      <c r="D21" s="67">
+        <v>545</v>
+      </c>
+      <c r="E21" s="67" t="s">
+        <v>159</v>
+      </c>
+      <c r="F21" s="67">
+        <v>21</v>
+      </c>
+      <c r="G21" s="67" t="s">
+        <v>160</v>
+      </c>
+      <c r="H21" s="67">
+        <v>13</v>
+      </c>
+      <c r="I21" s="67" t="s">
+        <v>90</v>
+      </c>
+      <c r="J21" s="67" t="s">
+        <v>179</v>
+      </c>
+      <c r="K21" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="L21" s="53" t="s">
+        <v>180</v>
+      </c>
+      <c r="M21" s="54"/>
+      <c r="N21" s="55"/>
+      <c r="O21" s="53" t="s">
+        <v>94</v>
+      </c>
+      <c r="P21" s="54"/>
+      <c r="Q21" s="55"/>
+    </row>
     <row r="22" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4943,15 +5196,19 @@
     <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="L18:N18"/>
-    <mergeCell ref="O18:Q18"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="O12:Q12"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="O13:Q13"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="O14:Q14"/>
+  <mergeCells count="40">
+    <mergeCell ref="L19:N19"/>
+    <mergeCell ref="O19:Q19"/>
+    <mergeCell ref="L20:N20"/>
+    <mergeCell ref="O20:Q20"/>
+    <mergeCell ref="L21:N21"/>
+    <mergeCell ref="O21:Q21"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="O11:Q11"/>
     <mergeCell ref="L7:N7"/>
     <mergeCell ref="O7:Q7"/>
     <mergeCell ref="L8:N8"/>
@@ -4966,12 +5223,14 @@
     <mergeCell ref="O4:Q4"/>
     <mergeCell ref="L5:N5"/>
     <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="O11:Q11"/>
+    <mergeCell ref="L18:N18"/>
+    <mergeCell ref="O18:Q18"/>
+    <mergeCell ref="L12:N12"/>
+    <mergeCell ref="O12:Q12"/>
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="O13:Q13"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="O14:Q14"/>
     <mergeCell ref="L15:N15"/>
     <mergeCell ref="O15:Q15"/>
     <mergeCell ref="L16:N16"/>

</xml_diff>